<commit_message>
Ajouts de tests pour le pitch schifter
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Plan de test integration.xlsx
+++ b/Documentation/Tests/Plan de test integration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippegosselin-bouchard/Documents/Ecole/Universite_de_Sherbrooke/S5/Projet/Repo/Documentation/Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olaberge\Documents\S5\Projet S5\Repo_Projet_S5\Documentation\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8F678A-E92B-D040-87EE-D395CCAA2F86}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8EA3FB-1FFE-4A0F-8D46-7B6A54AAF9FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="23540" activeTab="2" xr2:uid="{73256A17-FE39-444F-BF69-663F23F71EB5}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="182">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>Correlation et MAX(1) (Premier canal):</t>
-  </si>
-  <si>
-    <t>1.1.1</t>
   </si>
   <si>
     <t>2.1.1</t>
@@ -580,6 +577,15 @@
     <t xml:space="preserve">Phonème entré: I      Phonème identifié: 
 Phonème entré: OU Phonème identifié: 
 Phonème entré: U    Phonème identifié: </t>
+  </si>
+  <si>
+    <t>Entrée: Un signal de voix quelquonce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun bruit est entendu entre les trames </t>
+  </si>
+  <si>
+    <t>Le signal a une fréquence deux fois plus grande</t>
   </si>
 </sst>
 </file>
@@ -1445,6 +1451,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1657,18 +1666,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1681,39 +1690,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2034,71 +2040,71 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.6640625" customWidth="1"/>
-    <col min="15" max="15" width="29.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.6328125" customWidth="1"/>
+    <col min="15" max="15" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="F2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55"/>
-      <c r="F3" s="50" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="58"/>
+      <c r="F3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="60" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="61"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="64" t="s">
+      <c r="F5" s="64"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="65"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="68"/>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2109,193 +2115,193 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="68"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="71"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="O6" s="41"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O6" s="44"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="61"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="O7" s="42"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O7" s="45"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="58"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="61"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="42"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="45"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="58"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="61"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="42"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O9" s="45"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="61"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="42"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O10" s="45"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="61"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="42"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O11" s="45"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="61"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="42"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" s="45"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="58"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="61"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="42"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O13" s="45"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="61"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="O14" s="42"/>
-    </row>
-    <row r="15" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="45"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="53"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="56"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="O15" s="43"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="O15" s="46"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -2356,83 +2362,83 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="12" max="12" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="40" customWidth="1"/>
-    <col min="15" max="15" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="D2" s="48"/>
+      <c r="F2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="48" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="57">
         <v>1</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="58"/>
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
       <c r="L5" s="16" t="s">
         <v>7</v>
       </c>
@@ -2440,164 +2446,164 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="22">
         <v>1</v>
       </c>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="102"/>
-    </row>
-    <row r="7" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="105"/>
+    </row>
+    <row r="7" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="85" t="s">
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="94" t="s">
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="96"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="99"/>
       <c r="L7" s="20" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24">
         <v>1.2</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="109" t="s">
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="110"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="94" t="s">
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="95"/>
-      <c r="J8" s="95"/>
-      <c r="K8" s="96"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="99"/>
       <c r="L8" s="18" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:14" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="25">
         <v>1.3</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="89" t="s">
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="94" t="s">
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="96"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="99"/>
       <c r="L9" s="19" t="s">
         <v>18</v>
       </c>
       <c r="M9" s="21"/>
     </row>
-    <row r="10" spans="1:14" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="22">
         <v>2</v>
       </c>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="102"/>
-    </row>
-    <row r="11" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="105"/>
+    </row>
+    <row r="11" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23">
         <v>2.1</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="85" t="s">
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="94" t="s">
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="96"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="99"/>
       <c r="L11" s="20" t="s">
         <v>19</v>
       </c>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:14" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="87" t="s">
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="74" t="s">
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="76"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="79"/>
       <c r="L12" s="18" t="s">
         <v>19</v>
       </c>
@@ -2605,95 +2611,95 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="44.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="44.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="89" t="s">
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="91" t="s">
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="93"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="96"/>
       <c r="L13" s="19" t="s">
         <v>19</v>
       </c>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="1:14" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="22">
         <v>3</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="102"/>
-    </row>
-    <row r="15" spans="1:14" ht="56.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104"/>
+      <c r="L14" s="104"/>
+      <c r="M14" s="105"/>
+    </row>
+    <row r="15" spans="1:14" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23">
         <v>3.1</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="97" t="s">
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="94" t="s">
+      <c r="F15" s="101"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="96"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="99"/>
       <c r="L15" s="20" t="s">
         <v>19</v>
       </c>
       <c r="M15" s="30"/>
     </row>
-    <row r="16" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24">
         <v>3.2</v>
       </c>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="87" t="s">
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="74" t="s">
+      <c r="F16" s="91"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="76"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="79"/>
       <c r="L16" s="18" t="s">
         <v>19</v>
       </c>
@@ -2701,70 +2707,70 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="25">
         <v>3.3</v>
       </c>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="89" t="s">
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="91" t="s">
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="92"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="93"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="96"/>
       <c r="L17" s="19" t="s">
         <v>19</v>
       </c>
       <c r="M17" s="21"/>
     </row>
-    <row r="18" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="22">
         <v>4</v>
       </c>
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="101"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="102"/>
-    </row>
-    <row r="19" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="104"/>
+      <c r="L18" s="104"/>
+      <c r="M18" s="105"/>
+    </row>
+    <row r="19" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="26">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73" t="s">
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="77" t="s">
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
       <c r="L19" s="27" t="s">
         <v>19</v>
       </c>
@@ -2772,26 +2778,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="26">
         <v>4.3</v>
       </c>
-      <c r="B20" s="100" t="s">
+      <c r="B20" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="103" t="s">
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="104"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="106" t="s">
+      <c r="F20" s="107"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="109" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="107"/>
-      <c r="J20" s="107"/>
-      <c r="K20" s="108"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="111"/>
       <c r="L20" s="27" t="s">
         <v>19</v>
       </c>
@@ -2799,26 +2805,26 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="62" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="62" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="26">
         <v>4.2</v>
       </c>
-      <c r="B21" s="100" t="s">
+      <c r="B21" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73" t="s">
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="77" t="s">
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
       <c r="L21" s="27" t="s">
         <v>19</v>
       </c>
@@ -2826,22 +2832,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>14</v>
       </c>
@@ -2904,87 +2910,87 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD95B45-4342-44B1-A40B-F30FB3A286B9}">
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="137" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" customWidth="1"/>
+    <col min="12" max="12" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="D2" s="48"/>
+      <c r="F2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="48" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="57">
         <v>1</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="58"/>
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57" t="s">
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
       <c r="L5" s="32" t="s">
         <v>7</v>
       </c>
@@ -2992,1627 +2998,1634 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36">
         <v>1</v>
       </c>
-      <c r="B6" s="111" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-    </row>
-    <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="114" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+    </row>
+    <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
-    </row>
-    <row r="8" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="112"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="112"/>
-      <c r="K8" s="112"/>
+      <c r="B7" s="115" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="115" t="s">
+        <v>180</v>
+      </c>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="35"/>
+    </row>
+    <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B8" s="115" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115" t="s">
+        <v>181</v>
+      </c>
+      <c r="F8" s="115"/>
+      <c r="G8" s="115"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
       <c r="L8" s="35"/>
       <c r="M8" s="35"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36">
         <v>2</v>
       </c>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="111"/>
-      <c r="M9" s="111"/>
-    </row>
-    <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>2.1</v>
       </c>
-      <c r="B10" s="112" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="112"/>
-      <c r="J10" s="112"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
-    </row>
-    <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="115" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="115"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="112" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="112"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112" t="s">
-        <v>127</v>
-      </c>
-      <c r="F11" s="112"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="114" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="116"/>
+        <v>55</v>
+      </c>
+      <c r="B11" s="115" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" s="115"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="116" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="118"/>
       <c r="L11" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M11" s="33"/>
     </row>
-    <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="112" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="112"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="116"/>
+        <v>56</v>
+      </c>
+      <c r="B12" s="115" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="117"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="118"/>
       <c r="L12" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B13" s="112" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="112"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
-    </row>
-    <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="115" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="115"/>
+      <c r="L13" s="115"/>
+      <c r="M13" s="115"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="112" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="112"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" s="112"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="114" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" s="115"/>
-      <c r="J14" s="115"/>
-      <c r="K14" s="116"/>
+        <v>57</v>
+      </c>
+      <c r="B14" s="115" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="116" t="s">
+        <v>127</v>
+      </c>
+      <c r="I14" s="117"/>
+      <c r="J14" s="117"/>
+      <c r="K14" s="118"/>
       <c r="L14" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="112" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="115"/>
-      <c r="J15" s="115"/>
-      <c r="K15" s="116"/>
+        <v>58</v>
+      </c>
+      <c r="B15" s="115" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="117"/>
+      <c r="J15" s="117"/>
+      <c r="K15" s="118"/>
       <c r="L15" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M15" s="33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B16" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="112"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="112"/>
-      <c r="K16" s="112"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
-    </row>
-    <row r="17" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="115" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="115"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="115"/>
+      <c r="H16" s="115"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="115"/>
+      <c r="K16" s="115"/>
+      <c r="L16" s="115"/>
+      <c r="M16" s="115"/>
+    </row>
+    <row r="17" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="112" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="I17" s="115"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="116"/>
+        <v>59</v>
+      </c>
+      <c r="B17" s="115" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="115"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="116" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="117"/>
+      <c r="J17" s="117"/>
+      <c r="K17" s="118"/>
       <c r="L17" s="33" t="s">
         <v>19</v>
       </c>
       <c r="M17" s="33"/>
     </row>
-    <row r="18" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="I18" s="115"/>
-      <c r="J18" s="115"/>
-      <c r="K18" s="116"/>
+        <v>60</v>
+      </c>
+      <c r="B18" s="115" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="115"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="115"/>
+      <c r="G18" s="115"/>
+      <c r="H18" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" s="117"/>
+      <c r="J18" s="117"/>
+      <c r="K18" s="118"/>
       <c r="L18" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M18" s="33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="112" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="112"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="I19" s="115"/>
-      <c r="J19" s="115"/>
-      <c r="K19" s="116"/>
+        <v>72</v>
+      </c>
+      <c r="B19" s="115" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="117"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="118"/>
       <c r="L19" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M19" s="34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>2.4</v>
       </c>
-      <c r="B20" s="112" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="112"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
-    </row>
-    <row r="21" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="115" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="115"/>
+      <c r="D20" s="115"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="115"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="115"/>
+      <c r="K20" s="115"/>
+      <c r="L20" s="115"/>
+      <c r="M20" s="115"/>
+    </row>
+    <row r="21" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="112" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="112" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="114" t="s">
-        <v>117</v>
-      </c>
-      <c r="I21" s="115"/>
-      <c r="J21" s="115"/>
-      <c r="K21" s="116"/>
+        <v>61</v>
+      </c>
+      <c r="B21" s="115" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="115"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="116" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" s="117"/>
+      <c r="J21" s="117"/>
+      <c r="K21" s="118"/>
       <c r="L21" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M21" s="33"/>
     </row>
-    <row r="22" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="115"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="112"/>
-      <c r="G22" s="112"/>
-      <c r="H22" s="114" t="s">
-        <v>119</v>
-      </c>
-      <c r="I22" s="115"/>
-      <c r="J22" s="115"/>
-      <c r="K22" s="116"/>
+        <v>62</v>
+      </c>
+      <c r="B22" s="116" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" s="117"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="118"/>
       <c r="L22" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="115"/>
-      <c r="D23" s="116"/>
-      <c r="E23" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" s="112"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="114" t="s">
-        <v>118</v>
-      </c>
-      <c r="I23" s="115"/>
-      <c r="J23" s="115"/>
-      <c r="K23" s="116"/>
+        <v>76</v>
+      </c>
+      <c r="B23" s="116" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="117"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="115"/>
+      <c r="G23" s="115"/>
+      <c r="H23" s="116" t="s">
+        <v>117</v>
+      </c>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="118"/>
       <c r="L23" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M23" s="33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>2.5</v>
       </c>
-      <c r="B24" s="114" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="115"/>
-      <c r="D24" s="115"/>
-      <c r="E24" s="115"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="115"/>
-      <c r="H24" s="115"/>
-      <c r="I24" s="115"/>
-      <c r="J24" s="115"/>
-      <c r="K24" s="115"/>
-      <c r="L24" s="115"/>
-      <c r="M24" s="116"/>
-    </row>
-    <row r="25" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="116" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="117"/>
+      <c r="M24" s="118"/>
+    </row>
+    <row r="25" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="112"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="114" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" s="115"/>
-      <c r="J25" s="115"/>
-      <c r="K25" s="116"/>
+        <v>63</v>
+      </c>
+      <c r="B25" s="115" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="115"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="116" t="s">
+        <v>143</v>
+      </c>
+      <c r="I25" s="117"/>
+      <c r="J25" s="117"/>
+      <c r="K25" s="118"/>
       <c r="L25" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M25" s="33"/>
     </row>
-    <row r="26" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="114" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="115"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="I26" s="115"/>
-      <c r="J26" s="115"/>
-      <c r="K26" s="116"/>
+        <v>64</v>
+      </c>
+      <c r="B26" s="116" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="117"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="115"/>
+      <c r="G26" s="115"/>
+      <c r="H26" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" s="117"/>
+      <c r="J26" s="117"/>
+      <c r="K26" s="118"/>
       <c r="L26" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M26" s="33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="114" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="115"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F27" s="112"/>
-      <c r="G27" s="112"/>
-      <c r="H27" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="I27" s="115"/>
-      <c r="J27" s="115"/>
-      <c r="K27" s="116"/>
+        <v>73</v>
+      </c>
+      <c r="B27" s="116" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="117"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="118"/>
       <c r="L27" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M27" s="33" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18">
         <v>2.6</v>
       </c>
-      <c r="B28" s="112" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="112"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="112"/>
-      <c r="G28" s="112"/>
-      <c r="H28" s="112"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="112"/>
-      <c r="K28" s="112"/>
-      <c r="L28" s="112"/>
-      <c r="M28" s="112"/>
-    </row>
-    <row r="29" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="115" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="115"/>
+      <c r="D28" s="115"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="115"/>
+      <c r="G28" s="115"/>
+      <c r="H28" s="115"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="115"/>
+      <c r="M28" s="115"/>
+    </row>
+    <row r="29" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="112" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="112"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="114" t="s">
-        <v>145</v>
-      </c>
-      <c r="I29" s="115"/>
-      <c r="J29" s="115"/>
-      <c r="K29" s="116"/>
+        <v>65</v>
+      </c>
+      <c r="B29" s="115" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="115"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="115" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="115"/>
+      <c r="G29" s="115"/>
+      <c r="H29" s="116" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" s="117"/>
+      <c r="J29" s="117"/>
+      <c r="K29" s="118"/>
       <c r="L29" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M29" s="33"/>
     </row>
-    <row r="30" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="112" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="112"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" s="112"/>
-      <c r="G30" s="112"/>
-      <c r="H30" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="I30" s="115"/>
-      <c r="J30" s="115"/>
-      <c r="K30" s="116"/>
+        <v>66</v>
+      </c>
+      <c r="B30" s="115" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="115"/>
+      <c r="D30" s="115"/>
+      <c r="E30" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="115"/>
+      <c r="G30" s="115"/>
+      <c r="H30" s="116" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" s="117"/>
+      <c r="J30" s="117"/>
+      <c r="K30" s="118"/>
       <c r="L30" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>2.7</v>
       </c>
-      <c r="B31" s="112" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="112"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="112"/>
-      <c r="F31" s="112"/>
-      <c r="G31" s="112"/>
-      <c r="H31" s="112"/>
-      <c r="I31" s="112"/>
-      <c r="J31" s="112"/>
-      <c r="K31" s="112"/>
-      <c r="L31" s="112"/>
-      <c r="M31" s="112"/>
-    </row>
-    <row r="32" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="115" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="115"/>
+      <c r="D31" s="115"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="115"/>
+      <c r="G31" s="115"/>
+      <c r="H31" s="115"/>
+      <c r="I31" s="115"/>
+      <c r="J31" s="115"/>
+      <c r="K31" s="115"/>
+      <c r="L31" s="115"/>
+      <c r="M31" s="115"/>
+    </row>
+    <row r="32" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="112" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32" s="112"/>
-      <c r="D32" s="112"/>
-      <c r="E32" s="112" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="112"/>
-      <c r="G32" s="112"/>
-      <c r="H32" s="114" t="s">
-        <v>146</v>
-      </c>
-      <c r="I32" s="115"/>
-      <c r="J32" s="115"/>
-      <c r="K32" s="116"/>
+        <v>77</v>
+      </c>
+      <c r="B32" s="115" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="115"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="115" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" s="115"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="116" t="s">
+        <v>145</v>
+      </c>
+      <c r="I32" s="117"/>
+      <c r="J32" s="117"/>
+      <c r="K32" s="118"/>
       <c r="L32" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M32" s="33"/>
     </row>
-    <row r="33" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="112" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" s="112"/>
-      <c r="G33" s="112"/>
-      <c r="H33" s="114" t="s">
-        <v>130</v>
-      </c>
-      <c r="I33" s="115"/>
-      <c r="J33" s="115"/>
-      <c r="K33" s="116"/>
+        <v>78</v>
+      </c>
+      <c r="B33" s="115" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="115"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="115"/>
+      <c r="G33" s="115"/>
+      <c r="H33" s="116" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33" s="117"/>
+      <c r="J33" s="117"/>
+      <c r="K33" s="118"/>
       <c r="L33" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M33" s="33"/>
     </row>
-    <row r="34" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="37">
         <v>2.8</v>
       </c>
-      <c r="B34" s="113" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="113"/>
-      <c r="G34" s="113"/>
-      <c r="H34" s="113"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="113"/>
-      <c r="K34" s="113"/>
-      <c r="L34" s="113"/>
-      <c r="M34" s="113"/>
-    </row>
-    <row r="35" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="119" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="119"/>
+      <c r="D34" s="119"/>
+      <c r="E34" s="119"/>
+      <c r="F34" s="119"/>
+      <c r="G34" s="119"/>
+      <c r="H34" s="119"/>
+      <c r="I34" s="119"/>
+      <c r="J34" s="119"/>
+      <c r="K34" s="119"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="119"/>
+    </row>
+    <row r="35" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="120" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" s="120"/>
-      <c r="D35" s="120"/>
-      <c r="E35" s="120" t="s">
-        <v>147</v>
-      </c>
-      <c r="F35" s="120"/>
-      <c r="G35" s="120"/>
-      <c r="H35" s="117" t="s">
-        <v>151</v>
-      </c>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="119"/>
+        <v>85</v>
+      </c>
+      <c r="B35" s="123" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="123"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="123"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="120" t="s">
+        <v>150</v>
+      </c>
+      <c r="I35" s="121"/>
+      <c r="J35" s="121"/>
+      <c r="K35" s="122"/>
       <c r="L35" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M35" s="39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="120" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="123" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="123"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120" t="s">
-        <v>116</v>
-      </c>
-      <c r="F36" s="120"/>
-      <c r="G36" s="120"/>
-      <c r="H36" s="117" t="s">
-        <v>152</v>
-      </c>
-      <c r="I36" s="118"/>
-      <c r="J36" s="118"/>
-      <c r="K36" s="119"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="120" t="s">
+        <v>151</v>
+      </c>
+      <c r="I36" s="121"/>
+      <c r="J36" s="121"/>
+      <c r="K36" s="122"/>
       <c r="L36" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M36" s="39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="120" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" s="120"/>
-      <c r="D37" s="120"/>
-      <c r="E37" s="120" t="s">
-        <v>148</v>
-      </c>
-      <c r="F37" s="120"/>
-      <c r="G37" s="120"/>
-      <c r="H37" s="117" t="s">
-        <v>153</v>
-      </c>
-      <c r="I37" s="118"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="119"/>
+        <v>87</v>
+      </c>
+      <c r="B37" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="123"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="123" t="s">
+        <v>147</v>
+      </c>
+      <c r="F37" s="123"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="120" t="s">
+        <v>152</v>
+      </c>
+      <c r="I37" s="121"/>
+      <c r="J37" s="121"/>
+      <c r="K37" s="122"/>
       <c r="L37" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M37" s="39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18">
         <v>2.9</v>
       </c>
-      <c r="B38" s="112" t="s">
-        <v>133</v>
-      </c>
-      <c r="C38" s="112"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="112"/>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="112"/>
-      <c r="M38" s="112"/>
-    </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="115" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="115"/>
+      <c r="D38" s="115"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="115"/>
+      <c r="G38" s="115"/>
+      <c r="H38" s="115"/>
+      <c r="I38" s="115"/>
+      <c r="J38" s="115"/>
+      <c r="K38" s="115"/>
+      <c r="L38" s="115"/>
+      <c r="M38" s="115"/>
+    </row>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="112"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="114" t="s">
-        <v>127</v>
-      </c>
-      <c r="F39" s="115"/>
-      <c r="G39" s="116"/>
-      <c r="H39" s="114" t="s">
-        <v>154</v>
-      </c>
-      <c r="I39" s="115"/>
-      <c r="J39" s="115"/>
-      <c r="K39" s="116"/>
+        <v>88</v>
+      </c>
+      <c r="B39" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="115"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="116" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="117"/>
+      <c r="G39" s="118"/>
+      <c r="H39" s="116" t="s">
+        <v>153</v>
+      </c>
+      <c r="I39" s="117"/>
+      <c r="J39" s="117"/>
+      <c r="K39" s="118"/>
       <c r="L39" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M39" s="33"/>
     </row>
-    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="112"/>
-      <c r="D40" s="112"/>
-      <c r="E40" s="112" t="s">
-        <v>117</v>
-      </c>
-      <c r="F40" s="112"/>
-      <c r="G40" s="112"/>
-      <c r="H40" s="114" t="s">
-        <v>155</v>
-      </c>
-      <c r="I40" s="115"/>
-      <c r="J40" s="115"/>
-      <c r="K40" s="116"/>
+        <v>89</v>
+      </c>
+      <c r="B40" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="115"/>
+      <c r="D40" s="115"/>
+      <c r="E40" s="115" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="115"/>
+      <c r="G40" s="115"/>
+      <c r="H40" s="116" t="s">
+        <v>154</v>
+      </c>
+      <c r="I40" s="117"/>
+      <c r="J40" s="117"/>
+      <c r="K40" s="118"/>
       <c r="L40" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M40" s="33"/>
     </row>
-    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="112" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="114" t="s">
-        <v>145</v>
-      </c>
-      <c r="F41" s="115"/>
-      <c r="G41" s="116"/>
-      <c r="H41" s="114" t="s">
-        <v>156</v>
-      </c>
-      <c r="I41" s="115"/>
-      <c r="J41" s="115"/>
-      <c r="K41" s="116"/>
+        <v>90</v>
+      </c>
+      <c r="B41" s="115" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
+      <c r="E41" s="116" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="117"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="116" t="s">
+        <v>155</v>
+      </c>
+      <c r="I41" s="117"/>
+      <c r="J41" s="117"/>
+      <c r="K41" s="118"/>
       <c r="L41" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M41" s="33"/>
     </row>
-    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B42" s="112" t="s">
-        <v>134</v>
-      </c>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="112"/>
-      <c r="H42" s="112"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="112"/>
-      <c r="K42" s="112"/>
-      <c r="L42" s="112"/>
-      <c r="M42" s="112"/>
-    </row>
-    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="B42" s="115" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="115"/>
+      <c r="D42" s="115"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="115"/>
+      <c r="G42" s="115"/>
+      <c r="H42" s="115"/>
+      <c r="I42" s="115"/>
+      <c r="J42" s="115"/>
+      <c r="K42" s="115"/>
+      <c r="L42" s="115"/>
+      <c r="M42" s="115"/>
+    </row>
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112" t="s">
-        <v>128</v>
-      </c>
-      <c r="F43" s="112"/>
-      <c r="G43" s="112"/>
-      <c r="H43" s="114" t="s">
-        <v>157</v>
-      </c>
-      <c r="I43" s="115"/>
-      <c r="J43" s="115"/>
-      <c r="K43" s="116"/>
+        <v>91</v>
+      </c>
+      <c r="B43" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="115"/>
+      <c r="D43" s="115"/>
+      <c r="E43" s="115" t="s">
+        <v>127</v>
+      </c>
+      <c r="F43" s="115"/>
+      <c r="G43" s="115"/>
+      <c r="H43" s="116" t="s">
+        <v>156</v>
+      </c>
+      <c r="I43" s="117"/>
+      <c r="J43" s="117"/>
+      <c r="K43" s="118"/>
       <c r="L43" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M43" s="33"/>
     </row>
-    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="112" t="s">
-        <v>149</v>
-      </c>
-      <c r="F44" s="112"/>
-      <c r="G44" s="112"/>
-      <c r="H44" s="114" t="s">
-        <v>158</v>
-      </c>
-      <c r="I44" s="115"/>
-      <c r="J44" s="115"/>
-      <c r="K44" s="116"/>
+        <v>92</v>
+      </c>
+      <c r="B44" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="115"/>
+      <c r="D44" s="115"/>
+      <c r="E44" s="115" t="s">
+        <v>148</v>
+      </c>
+      <c r="F44" s="115"/>
+      <c r="G44" s="115"/>
+      <c r="H44" s="116" t="s">
+        <v>157</v>
+      </c>
+      <c r="I44" s="117"/>
+      <c r="J44" s="117"/>
+      <c r="K44" s="118"/>
       <c r="L44" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M44" s="33"/>
     </row>
-    <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" s="112" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" s="112"/>
-      <c r="D45" s="112"/>
-      <c r="E45" s="112" t="s">
-        <v>150</v>
-      </c>
-      <c r="F45" s="112"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="114" t="s">
-        <v>159</v>
-      </c>
-      <c r="I45" s="115"/>
-      <c r="J45" s="115"/>
-      <c r="K45" s="116"/>
+        <v>93</v>
+      </c>
+      <c r="B45" s="115" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="115"/>
+      <c r="D45" s="115"/>
+      <c r="E45" s="115" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" s="115"/>
+      <c r="G45" s="115"/>
+      <c r="H45" s="116" t="s">
+        <v>158</v>
+      </c>
+      <c r="I45" s="117"/>
+      <c r="J45" s="117"/>
+      <c r="K45" s="118"/>
       <c r="L45" s="34" t="s">
         <v>19</v>
       </c>
       <c r="M45" s="33"/>
     </row>
-    <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18">
         <v>2.11</v>
       </c>
-      <c r="B46" s="112" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" s="112"/>
-      <c r="D46" s="112"/>
-      <c r="E46" s="112"/>
-      <c r="F46" s="112"/>
-      <c r="G46" s="112"/>
-      <c r="H46" s="112"/>
-      <c r="I46" s="112"/>
-      <c r="J46" s="112"/>
-      <c r="K46" s="112"/>
-      <c r="L46" s="112"/>
-      <c r="M46" s="112"/>
-    </row>
-    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="115" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="115"/>
+      <c r="D46" s="115"/>
+      <c r="E46" s="115"/>
+      <c r="F46" s="115"/>
+      <c r="G46" s="115"/>
+      <c r="H46" s="115"/>
+      <c r="I46" s="115"/>
+      <c r="J46" s="115"/>
+      <c r="K46" s="115"/>
+      <c r="L46" s="115"/>
+      <c r="M46" s="115"/>
+    </row>
+    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="112"/>
-      <c r="D47" s="112"/>
-      <c r="E47" s="114" t="s">
-        <v>127</v>
-      </c>
-      <c r="F47" s="115"/>
-      <c r="G47" s="116"/>
-      <c r="H47" s="114" t="s">
-        <v>164</v>
-      </c>
-      <c r="I47" s="115"/>
-      <c r="J47" s="115"/>
-      <c r="K47" s="116"/>
+        <v>134</v>
+      </c>
+      <c r="B47" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="115"/>
+      <c r="D47" s="115"/>
+      <c r="E47" s="116" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="117"/>
+      <c r="G47" s="118"/>
+      <c r="H47" s="116" t="s">
+        <v>163</v>
+      </c>
+      <c r="I47" s="117"/>
+      <c r="J47" s="117"/>
+      <c r="K47" s="118"/>
       <c r="L47" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M47" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B48" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="112"/>
-      <c r="E48" s="112" t="s">
-        <v>149</v>
-      </c>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="114" t="s">
-        <v>158</v>
-      </c>
-      <c r="I48" s="115"/>
-      <c r="J48" s="115"/>
-      <c r="K48" s="116"/>
+        <v>135</v>
+      </c>
+      <c r="B48" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="115"/>
+      <c r="D48" s="115"/>
+      <c r="E48" s="115" t="s">
+        <v>148</v>
+      </c>
+      <c r="F48" s="115"/>
+      <c r="G48" s="115"/>
+      <c r="H48" s="116" t="s">
+        <v>157</v>
+      </c>
+      <c r="I48" s="117"/>
+      <c r="J48" s="117"/>
+      <c r="K48" s="118"/>
       <c r="L48" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M48" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B49" s="112" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" s="112"/>
-      <c r="D49" s="112"/>
-      <c r="E49" s="114" t="s">
-        <v>150</v>
-      </c>
-      <c r="F49" s="115"/>
-      <c r="G49" s="116"/>
-      <c r="H49" s="114" t="s">
-        <v>159</v>
-      </c>
-      <c r="I49" s="115"/>
-      <c r="J49" s="115"/>
-      <c r="K49" s="116"/>
+        <v>136</v>
+      </c>
+      <c r="B49" s="115" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="115"/>
+      <c r="D49" s="115"/>
+      <c r="E49" s="116" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49" s="117"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="116" t="s">
+        <v>158</v>
+      </c>
+      <c r="I49" s="117"/>
+      <c r="J49" s="117"/>
+      <c r="K49" s="118"/>
       <c r="L49" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M49" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18">
         <v>2.12</v>
       </c>
-      <c r="B50" s="114" t="s">
-        <v>161</v>
-      </c>
-      <c r="C50" s="115"/>
-      <c r="D50" s="115"/>
-      <c r="E50" s="115"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="115"/>
-      <c r="H50" s="115"/>
-      <c r="I50" s="115"/>
-      <c r="J50" s="115"/>
-      <c r="K50" s="115"/>
-      <c r="L50" s="115"/>
-      <c r="M50" s="116"/>
-    </row>
-    <row r="51" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="116" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="117"/>
+      <c r="D50" s="117"/>
+      <c r="E50" s="117"/>
+      <c r="F50" s="117"/>
+      <c r="G50" s="117"/>
+      <c r="H50" s="117"/>
+      <c r="I50" s="117"/>
+      <c r="J50" s="117"/>
+      <c r="K50" s="117"/>
+      <c r="L50" s="117"/>
+      <c r="M50" s="118"/>
+    </row>
+    <row r="51" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B51" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="112"/>
-      <c r="D51" s="112"/>
-      <c r="E51" s="114" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" s="115"/>
-      <c r="G51" s="116"/>
-      <c r="H51" s="114" t="s">
-        <v>157</v>
-      </c>
-      <c r="I51" s="115"/>
-      <c r="J51" s="115"/>
-      <c r="K51" s="116"/>
+        <v>137</v>
+      </c>
+      <c r="B51" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="115"/>
+      <c r="D51" s="115"/>
+      <c r="E51" s="116" t="s">
+        <v>127</v>
+      </c>
+      <c r="F51" s="117"/>
+      <c r="G51" s="118"/>
+      <c r="H51" s="116" t="s">
+        <v>156</v>
+      </c>
+      <c r="I51" s="117"/>
+      <c r="J51" s="117"/>
+      <c r="K51" s="118"/>
       <c r="L51" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M51" s="38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="115"/>
+      <c r="D52" s="115"/>
+      <c r="E52" s="115" t="s">
+        <v>116</v>
+      </c>
+      <c r="F52" s="115"/>
+      <c r="G52" s="115"/>
+      <c r="H52" s="116" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B52" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="112"/>
-      <c r="D52" s="112"/>
-      <c r="E52" s="112" t="s">
-        <v>117</v>
-      </c>
-      <c r="F52" s="112"/>
-      <c r="G52" s="112"/>
-      <c r="H52" s="114" t="s">
-        <v>166</v>
-      </c>
-      <c r="I52" s="115"/>
-      <c r="J52" s="115"/>
-      <c r="K52" s="116"/>
+      <c r="I52" s="117"/>
+      <c r="J52" s="117"/>
+      <c r="K52" s="118"/>
       <c r="L52" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M52" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="B53" s="112" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="112"/>
-      <c r="D53" s="112"/>
-      <c r="E53" s="114" t="s">
-        <v>150</v>
-      </c>
-      <c r="F53" s="115"/>
-      <c r="G53" s="116"/>
-      <c r="H53" s="114" t="s">
-        <v>159</v>
-      </c>
-      <c r="I53" s="115"/>
-      <c r="J53" s="115"/>
-      <c r="K53" s="116"/>
+        <v>139</v>
+      </c>
+      <c r="B53" s="115" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="115"/>
+      <c r="D53" s="115"/>
+      <c r="E53" s="116" t="s">
+        <v>149</v>
+      </c>
+      <c r="F53" s="117"/>
+      <c r="G53" s="118"/>
+      <c r="H53" s="116" t="s">
+        <v>158</v>
+      </c>
+      <c r="I53" s="117"/>
+      <c r="J53" s="117"/>
+      <c r="K53" s="118"/>
       <c r="L53" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M53" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18">
         <v>2.13</v>
       </c>
-      <c r="B54" s="112" t="s">
-        <v>162</v>
-      </c>
-      <c r="C54" s="112"/>
-      <c r="D54" s="112"/>
-      <c r="E54" s="112"/>
-      <c r="F54" s="112"/>
-      <c r="G54" s="112"/>
-      <c r="H54" s="112"/>
-      <c r="I54" s="112"/>
-      <c r="J54" s="112"/>
-      <c r="K54" s="112"/>
-      <c r="L54" s="112"/>
-      <c r="M54" s="112"/>
-    </row>
-    <row r="55" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="115" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" s="115"/>
+      <c r="D54" s="115"/>
+      <c r="E54" s="115"/>
+      <c r="F54" s="115"/>
+      <c r="G54" s="115"/>
+      <c r="H54" s="115"/>
+      <c r="I54" s="115"/>
+      <c r="J54" s="115"/>
+      <c r="K54" s="115"/>
+      <c r="L54" s="115"/>
+      <c r="M54" s="115"/>
+    </row>
+    <row r="55" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B55" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" s="112"/>
-      <c r="D55" s="112"/>
-      <c r="E55" s="114" t="s">
-        <v>128</v>
-      </c>
-      <c r="F55" s="115"/>
-      <c r="G55" s="116"/>
-      <c r="H55" s="114" t="s">
-        <v>157</v>
-      </c>
-      <c r="I55" s="115"/>
-      <c r="J55" s="115"/>
-      <c r="K55" s="116"/>
+        <v>140</v>
+      </c>
+      <c r="B55" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="115"/>
+      <c r="D55" s="115"/>
+      <c r="E55" s="116" t="s">
+        <v>127</v>
+      </c>
+      <c r="F55" s="117"/>
+      <c r="G55" s="118"/>
+      <c r="H55" s="116" t="s">
+        <v>156</v>
+      </c>
+      <c r="I55" s="117"/>
+      <c r="J55" s="117"/>
+      <c r="K55" s="118"/>
       <c r="L55" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M55" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B56" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="112"/>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112" t="s">
-        <v>149</v>
-      </c>
-      <c r="F56" s="112"/>
-      <c r="G56" s="112"/>
-      <c r="H56" s="114" t="s">
-        <v>158</v>
-      </c>
-      <c r="I56" s="115"/>
-      <c r="J56" s="115"/>
-      <c r="K56" s="116"/>
+        <v>141</v>
+      </c>
+      <c r="B56" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="115"/>
+      <c r="D56" s="115"/>
+      <c r="E56" s="115" t="s">
+        <v>148</v>
+      </c>
+      <c r="F56" s="115"/>
+      <c r="G56" s="115"/>
+      <c r="H56" s="116" t="s">
+        <v>157</v>
+      </c>
+      <c r="I56" s="117"/>
+      <c r="J56" s="117"/>
+      <c r="K56" s="118"/>
       <c r="L56" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M56" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B57" s="112" t="s">
-        <v>129</v>
-      </c>
-      <c r="C57" s="112"/>
-      <c r="D57" s="112"/>
-      <c r="E57" s="114" t="s">
-        <v>145</v>
-      </c>
-      <c r="F57" s="115"/>
-      <c r="G57" s="116"/>
-      <c r="H57" s="114" t="s">
-        <v>167</v>
-      </c>
-      <c r="I57" s="115"/>
-      <c r="J57" s="115"/>
-      <c r="K57" s="116"/>
+        <v>142</v>
+      </c>
+      <c r="B57" s="115" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="115"/>
+      <c r="D57" s="115"/>
+      <c r="E57" s="116" t="s">
+        <v>144</v>
+      </c>
+      <c r="F57" s="117"/>
+      <c r="G57" s="118"/>
+      <c r="H57" s="116" t="s">
+        <v>166</v>
+      </c>
+      <c r="I57" s="117"/>
+      <c r="J57" s="117"/>
+      <c r="K57" s="118"/>
       <c r="L57" s="38" t="s">
         <v>19</v>
       </c>
       <c r="M57" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="36">
         <v>3</v>
       </c>
-      <c r="B58" s="111" t="s">
+      <c r="B58" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="111"/>
-      <c r="D58" s="111"/>
-      <c r="E58" s="111"/>
-      <c r="F58" s="111"/>
-      <c r="G58" s="111"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
-      <c r="J58" s="111"/>
-      <c r="K58" s="111"/>
-      <c r="L58" s="111"/>
-      <c r="M58" s="111"/>
-    </row>
-    <row r="59" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="114"/>
+      <c r="D58" s="114"/>
+      <c r="E58" s="114"/>
+      <c r="F58" s="114"/>
+      <c r="G58" s="114"/>
+      <c r="H58" s="114"/>
+      <c r="I58" s="114"/>
+      <c r="J58" s="114"/>
+      <c r="K58" s="114"/>
+      <c r="L58" s="114"/>
+      <c r="M58" s="114"/>
+    </row>
+    <row r="59" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="18">
         <v>3.1</v>
       </c>
-      <c r="B59" s="112" t="s">
+      <c r="B59" s="115" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="112"/>
-      <c r="D59" s="112"/>
-      <c r="E59" s="112"/>
-      <c r="F59" s="112"/>
-      <c r="G59" s="112"/>
-      <c r="H59" s="112"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="112"/>
-      <c r="L59" s="112"/>
-      <c r="M59" s="112"/>
-    </row>
-    <row r="60" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="115"/>
+      <c r="D59" s="115"/>
+      <c r="E59" s="115"/>
+      <c r="F59" s="115"/>
+      <c r="G59" s="115"/>
+      <c r="H59" s="115"/>
+      <c r="I59" s="115"/>
+      <c r="J59" s="115"/>
+      <c r="K59" s="115"/>
+      <c r="L59" s="115"/>
+      <c r="M59" s="115"/>
+    </row>
+    <row r="60" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="114" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="115"/>
-      <c r="D60" s="116"/>
-      <c r="E60" s="114" t="s">
-        <v>97</v>
-      </c>
-      <c r="F60" s="115"/>
-      <c r="G60" s="116"/>
-      <c r="H60" s="114"/>
-      <c r="I60" s="115"/>
-      <c r="J60" s="115"/>
-      <c r="K60" s="116"/>
+        <v>67</v>
+      </c>
+      <c r="B60" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="117"/>
+      <c r="D60" s="118"/>
+      <c r="E60" s="116" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="117"/>
+      <c r="G60" s="118"/>
+      <c r="H60" s="116"/>
+      <c r="I60" s="117"/>
+      <c r="J60" s="117"/>
+      <c r="K60" s="118"/>
       <c r="L60" s="33"/>
       <c r="M60" s="33"/>
     </row>
-    <row r="61" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="18">
         <v>3.2</v>
       </c>
-      <c r="B61" s="112" t="s">
+      <c r="B61" s="115" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="115"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="115"/>
+      <c r="G61" s="115"/>
+      <c r="H61" s="115"/>
+      <c r="I61" s="115"/>
+      <c r="J61" s="115"/>
+      <c r="K61" s="115"/>
+      <c r="L61" s="115"/>
+      <c r="M61" s="115"/>
+    </row>
+    <row r="62" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="C61" s="112"/>
-      <c r="D61" s="112"/>
-      <c r="E61" s="112"/>
-      <c r="F61" s="112"/>
-      <c r="G61" s="112"/>
-      <c r="H61" s="112"/>
-      <c r="I61" s="112"/>
-      <c r="J61" s="112"/>
-      <c r="K61" s="112"/>
-      <c r="L61" s="112"/>
-      <c r="M61" s="112"/>
-    </row>
-    <row r="62" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B62" s="114" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" s="115"/>
-      <c r="D62" s="116"/>
-      <c r="E62" s="114" t="s">
-        <v>98</v>
-      </c>
-      <c r="F62" s="115"/>
-      <c r="G62" s="116"/>
-      <c r="H62" s="114"/>
-      <c r="I62" s="115"/>
-      <c r="J62" s="115"/>
-      <c r="K62" s="116"/>
+      <c r="C62" s="117"/>
+      <c r="D62" s="118"/>
+      <c r="E62" s="116" t="s">
+        <v>97</v>
+      </c>
+      <c r="F62" s="117"/>
+      <c r="G62" s="118"/>
+      <c r="H62" s="116"/>
+      <c r="I62" s="117"/>
+      <c r="J62" s="117"/>
+      <c r="K62" s="118"/>
       <c r="L62" s="33"/>
       <c r="M62" s="33"/>
     </row>
-    <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="18">
         <v>3.3</v>
       </c>
-      <c r="B63" s="112" t="s">
+      <c r="B63" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="112"/>
-      <c r="D63" s="112"/>
-      <c r="E63" s="112"/>
-      <c r="F63" s="112"/>
-      <c r="G63" s="112"/>
-      <c r="H63" s="112"/>
-      <c r="I63" s="112"/>
-      <c r="J63" s="112"/>
-      <c r="K63" s="112"/>
-      <c r="L63" s="112"/>
-      <c r="M63" s="112"/>
-    </row>
-    <row r="64" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="115"/>
+      <c r="D63" s="115"/>
+      <c r="E63" s="115"/>
+      <c r="F63" s="115"/>
+      <c r="G63" s="115"/>
+      <c r="H63" s="115"/>
+      <c r="I63" s="115"/>
+      <c r="J63" s="115"/>
+      <c r="K63" s="115"/>
+      <c r="L63" s="115"/>
+      <c r="M63" s="115"/>
+    </row>
+    <row r="64" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="114" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="115"/>
-      <c r="D64" s="116"/>
-      <c r="E64" s="114" t="s">
-        <v>97</v>
-      </c>
-      <c r="F64" s="115"/>
-      <c r="G64" s="116"/>
-      <c r="H64" s="114"/>
-      <c r="I64" s="115"/>
-      <c r="J64" s="115"/>
-      <c r="K64" s="116"/>
+        <v>69</v>
+      </c>
+      <c r="B64" s="116" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="117"/>
+      <c r="D64" s="118"/>
+      <c r="E64" s="116" t="s">
+        <v>96</v>
+      </c>
+      <c r="F64" s="117"/>
+      <c r="G64" s="118"/>
+      <c r="H64" s="116"/>
+      <c r="I64" s="117"/>
+      <c r="J64" s="117"/>
+      <c r="K64" s="118"/>
       <c r="L64" s="33"/>
       <c r="M64" s="33"/>
     </row>
-    <row r="65" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B65" s="114" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="115"/>
-      <c r="D65" s="116"/>
-      <c r="E65" s="114" t="s">
-        <v>75</v>
-      </c>
-      <c r="F65" s="115"/>
-      <c r="G65" s="116"/>
-      <c r="H65" s="114"/>
-      <c r="I65" s="115"/>
-      <c r="J65" s="115"/>
-      <c r="K65" s="116"/>
+        <v>70</v>
+      </c>
+      <c r="B65" s="116" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="117"/>
+      <c r="D65" s="118"/>
+      <c r="E65" s="116" t="s">
+        <v>74</v>
+      </c>
+      <c r="F65" s="117"/>
+      <c r="G65" s="118"/>
+      <c r="H65" s="116"/>
+      <c r="I65" s="117"/>
+      <c r="J65" s="117"/>
+      <c r="K65" s="118"/>
       <c r="L65" s="40"/>
       <c r="M65" s="40"/>
     </row>
-    <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="18">
         <v>4</v>
       </c>
-      <c r="B66" s="116" t="s">
-        <v>168</v>
-      </c>
-      <c r="C66" s="112"/>
-      <c r="D66" s="112"/>
-      <c r="E66" s="112"/>
-      <c r="F66" s="112"/>
-      <c r="G66" s="112"/>
-      <c r="H66" s="112"/>
-      <c r="I66" s="112"/>
-      <c r="J66" s="112"/>
-      <c r="K66" s="112"/>
-      <c r="L66" s="112"/>
-      <c r="M66" s="112"/>
-    </row>
-    <row r="67" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" s="115"/>
+      <c r="D66" s="115"/>
+      <c r="E66" s="115"/>
+      <c r="F66" s="115"/>
+      <c r="G66" s="115"/>
+      <c r="H66" s="115"/>
+      <c r="I66" s="115"/>
+      <c r="J66" s="115"/>
+      <c r="K66" s="115"/>
+      <c r="L66" s="115"/>
+      <c r="M66" s="115"/>
+    </row>
+    <row r="67" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B67" s="114" t="s">
-        <v>171</v>
-      </c>
-      <c r="C67" s="115"/>
-      <c r="D67" s="116"/>
-      <c r="E67" s="114" t="s">
-        <v>169</v>
-      </c>
-      <c r="F67" s="115"/>
-      <c r="G67" s="116"/>
-      <c r="H67" s="114" t="s">
-        <v>178</v>
-      </c>
-      <c r="I67" s="129"/>
-      <c r="J67" s="129"/>
-      <c r="K67" s="130"/>
-      <c r="L67" s="128"/>
-      <c r="M67" s="124"/>
-    </row>
-    <row r="68" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="116" t="s">
+        <v>170</v>
+      </c>
+      <c r="C67" s="117"/>
+      <c r="D67" s="118"/>
+      <c r="E67" s="116" t="s">
+        <v>168</v>
+      </c>
+      <c r="F67" s="117"/>
+      <c r="G67" s="118"/>
+      <c r="H67" s="116" t="s">
+        <v>177</v>
+      </c>
+      <c r="I67" s="124"/>
+      <c r="J67" s="124"/>
+      <c r="K67" s="125"/>
+      <c r="L67" s="42"/>
+      <c r="M67" s="41"/>
+    </row>
+    <row r="68" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="18">
         <v>4.2</v>
       </c>
-      <c r="B68" s="122" t="s">
-        <v>172</v>
-      </c>
-      <c r="C68" s="121"/>
-      <c r="D68" s="123"/>
-      <c r="E68" s="122" t="s">
-        <v>169</v>
-      </c>
-      <c r="F68" s="121"/>
-      <c r="G68" s="123"/>
-      <c r="H68" s="114" t="s">
-        <v>178</v>
-      </c>
-      <c r="I68" s="129"/>
-      <c r="J68" s="129"/>
-      <c r="K68" s="130"/>
-      <c r="L68" s="128"/>
-      <c r="M68" s="124"/>
-    </row>
-    <row r="69" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="126" t="s">
+        <v>171</v>
+      </c>
+      <c r="C68" s="127"/>
+      <c r="D68" s="128"/>
+      <c r="E68" s="126" t="s">
+        <v>168</v>
+      </c>
+      <c r="F68" s="127"/>
+      <c r="G68" s="128"/>
+      <c r="H68" s="116" t="s">
+        <v>177</v>
+      </c>
+      <c r="I68" s="124"/>
+      <c r="J68" s="124"/>
+      <c r="K68" s="125"/>
+      <c r="L68" s="42"/>
+      <c r="M68" s="41"/>
+    </row>
+    <row r="69" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="18">
         <v>4.3</v>
       </c>
-      <c r="B69" s="126" t="s">
-        <v>173</v>
-      </c>
-      <c r="C69" s="125"/>
-      <c r="D69" s="127"/>
-      <c r="E69" s="122" t="s">
-        <v>169</v>
-      </c>
-      <c r="F69" s="121"/>
-      <c r="G69" s="123"/>
-      <c r="H69" s="114" t="s">
-        <v>178</v>
-      </c>
-      <c r="I69" s="129"/>
-      <c r="J69" s="129"/>
-      <c r="K69" s="130"/>
-      <c r="L69" s="128"/>
-      <c r="M69" s="124"/>
-    </row>
-    <row r="70" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="129" t="s">
+        <v>172</v>
+      </c>
+      <c r="C69" s="130"/>
+      <c r="D69" s="131"/>
+      <c r="E69" s="126" t="s">
+        <v>168</v>
+      </c>
+      <c r="F69" s="127"/>
+      <c r="G69" s="128"/>
+      <c r="H69" s="116" t="s">
+        <v>177</v>
+      </c>
+      <c r="I69" s="124"/>
+      <c r="J69" s="124"/>
+      <c r="K69" s="125"/>
+      <c r="L69" s="42"/>
+      <c r="M69" s="41"/>
+    </row>
+    <row r="70" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="18">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B70" s="126" t="s">
-        <v>174</v>
-      </c>
-      <c r="C70" s="125"/>
-      <c r="D70" s="127"/>
-      <c r="E70" s="122" t="s">
-        <v>169</v>
-      </c>
-      <c r="F70" s="121"/>
-      <c r="G70" s="123"/>
-      <c r="H70" s="114" t="s">
-        <v>178</v>
-      </c>
-      <c r="I70" s="129"/>
-      <c r="J70" s="129"/>
-      <c r="K70" s="130"/>
-      <c r="L70" s="128"/>
-      <c r="M70" s="124"/>
-    </row>
-    <row r="71" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="129" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" s="130"/>
+      <c r="D70" s="131"/>
+      <c r="E70" s="126" t="s">
+        <v>168</v>
+      </c>
+      <c r="F70" s="127"/>
+      <c r="G70" s="128"/>
+      <c r="H70" s="116" t="s">
+        <v>177</v>
+      </c>
+      <c r="I70" s="124"/>
+      <c r="J70" s="124"/>
+      <c r="K70" s="125"/>
+      <c r="L70" s="42"/>
+      <c r="M70" s="41"/>
+    </row>
+    <row r="71" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18">
         <v>4.5</v>
       </c>
-      <c r="B71" s="122" t="s">
-        <v>175</v>
-      </c>
-      <c r="C71" s="121"/>
-      <c r="D71" s="123"/>
-      <c r="E71" s="114" t="s">
-        <v>170</v>
-      </c>
-      <c r="F71" s="115"/>
-      <c r="G71" s="116"/>
-      <c r="H71" s="122" t="s">
-        <v>179</v>
-      </c>
-      <c r="I71" s="131"/>
-      <c r="J71" s="131"/>
-      <c r="K71" s="132"/>
-      <c r="L71" s="128"/>
-      <c r="M71" s="124"/>
-    </row>
-    <row r="72" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="126" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" s="127"/>
+      <c r="D71" s="128"/>
+      <c r="E71" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="F71" s="117"/>
+      <c r="G71" s="118"/>
+      <c r="H71" s="126" t="s">
+        <v>178</v>
+      </c>
+      <c r="I71" s="132"/>
+      <c r="J71" s="132"/>
+      <c r="K71" s="133"/>
+      <c r="L71" s="42"/>
+      <c r="M71" s="41"/>
+    </row>
+    <row r="72" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="18">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B72" s="114" t="s">
-        <v>176</v>
-      </c>
-      <c r="C72" s="115"/>
-      <c r="D72" s="116"/>
-      <c r="E72" s="114" t="s">
-        <v>170</v>
-      </c>
-      <c r="F72" s="115"/>
-      <c r="G72" s="116"/>
-      <c r="H72" s="121" t="s">
-        <v>179</v>
-      </c>
-      <c r="I72" s="131"/>
-      <c r="J72" s="131"/>
-      <c r="K72" s="132"/>
-      <c r="L72" s="128"/>
-      <c r="M72" s="124"/>
-    </row>
-    <row r="73" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="116" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" s="117"/>
+      <c r="D72" s="118"/>
+      <c r="E72" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="F72" s="117"/>
+      <c r="G72" s="118"/>
+      <c r="H72" s="127" t="s">
+        <v>178</v>
+      </c>
+      <c r="I72" s="132"/>
+      <c r="J72" s="132"/>
+      <c r="K72" s="133"/>
+      <c r="L72" s="42"/>
+      <c r="M72" s="41"/>
+    </row>
+    <row r="73" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="18">
         <v>4.7</v>
       </c>
-      <c r="B73" s="126" t="s">
-        <v>177</v>
-      </c>
-      <c r="C73" s="125"/>
-      <c r="D73" s="127"/>
-      <c r="E73" s="114" t="s">
-        <v>170</v>
-      </c>
-      <c r="F73" s="115"/>
-      <c r="G73" s="116"/>
-      <c r="H73" s="121" t="s">
-        <v>179</v>
-      </c>
-      <c r="I73" s="131"/>
-      <c r="J73" s="131"/>
-      <c r="K73" s="132"/>
-      <c r="L73" s="128"/>
-      <c r="M73" s="124"/>
-    </row>
-    <row r="74" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="129" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" s="130"/>
+      <c r="D73" s="131"/>
+      <c r="E73" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="F73" s="117"/>
+      <c r="G73" s="118"/>
+      <c r="H73" s="127" t="s">
+        <v>178</v>
+      </c>
+      <c r="I73" s="132"/>
+      <c r="J73" s="132"/>
+      <c r="K73" s="133"/>
+      <c r="L73" s="42"/>
+      <c r="M73" s="41"/>
+    </row>
+    <row r="74" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="18">
         <v>4.8</v>
       </c>
-      <c r="B74" s="126" t="s">
-        <v>176</v>
-      </c>
-      <c r="C74" s="125"/>
-      <c r="D74" s="127"/>
-      <c r="E74" s="122" t="s">
-        <v>170</v>
-      </c>
-      <c r="F74" s="121"/>
-      <c r="G74" s="123"/>
-      <c r="H74" s="121" t="s">
-        <v>179</v>
-      </c>
-      <c r="I74" s="131"/>
-      <c r="J74" s="131"/>
-      <c r="K74" s="132"/>
-      <c r="L74" s="128"/>
-      <c r="M74" s="124"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E75" s="133"/>
-      <c r="F75" s="133"/>
-      <c r="G75" s="133"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E76" s="133"/>
-      <c r="F76" s="133"/>
-      <c r="G76" s="133"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
+      <c r="B74" s="129" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="130"/>
+      <c r="D74" s="131"/>
+      <c r="E74" s="126" t="s">
+        <v>169</v>
+      </c>
+      <c r="F74" s="127"/>
+      <c r="G74" s="128"/>
+      <c r="H74" s="127" t="s">
+        <v>178</v>
+      </c>
+      <c r="I74" s="132"/>
+      <c r="J74" s="132"/>
+      <c r="K74" s="133"/>
+      <c r="L74" s="42"/>
+      <c r="M74" s="41"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="174">
+  <mergeCells count="176">
     <mergeCell ref="B73:D73"/>
     <mergeCell ref="E73:G73"/>
     <mergeCell ref="H73:K73"/>
@@ -4747,15 +4760,14 @@
     <mergeCell ref="B59:M59"/>
     <mergeCell ref="B61:M61"/>
     <mergeCell ref="B63:M63"/>
-    <mergeCell ref="B7:M7"/>
     <mergeCell ref="B10:M10"/>
     <mergeCell ref="B28:M28"/>
     <mergeCell ref="B38:M38"/>
     <mergeCell ref="B58:M58"/>
     <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:K7"/>
     <mergeCell ref="B16:M16"/>
     <mergeCell ref="B20:M20"/>
     <mergeCell ref="B34:M34"/>
@@ -4787,6 +4799,9 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="H15:K15"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Retour sur l'assurance qualité
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Plan de test integration.xlsx
+++ b/Documentation/Tests/Plan de test integration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olaberge\Documents\S5\Projet S5\Repo_Projet_S5\Documentation\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8EA3FB-1FFE-4A0F-8D46-7B6A54AAF9FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44984611-9897-4D87-BAAD-F32662B8BB9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="23540" activeTab="2" xr2:uid="{73256A17-FE39-444F-BF69-663F23F71EB5}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="182">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -1454,6 +1454,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1483,72 +1537,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1558,48 +1651,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1609,116 +1660,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2053,16 +2053,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="70"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2071,16 +2071,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58"/>
-      <c r="F3" s="53" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
+      <c r="F3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2089,22 +2089,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="63" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="67" t="s">
+      <c r="F5" s="45"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="68"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="46"/>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2119,181 +2119,181 @@
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="59"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="O6" s="44"/>
+      <c r="O6" s="62"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="61"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
       <c r="K7" s="61"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="O7" s="45"/>
+      <c r="O7" s="63"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="61"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
       <c r="K8" s="61"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="45"/>
+      <c r="O8" s="63"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="51"/>
       <c r="D9" s="61"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
       <c r="K9" s="61"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="45"/>
+      <c r="O9" s="63"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="61"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
       <c r="K10" s="61"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="45"/>
+      <c r="O10" s="63"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="61"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
       <c r="K11" s="61"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="45"/>
+      <c r="O11" s="63"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="60"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="61"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
       <c r="K12" s="61"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="45"/>
+      <c r="O12" s="63"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="61"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
       <c r="K13" s="61"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="45"/>
+      <c r="O13" s="63"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="60"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="61"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
       <c r="K14" s="61"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="O14" s="45"/>
+      <c r="O14" s="63"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="56"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="O15" s="46"/>
+      <c r="O15" s="64"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -2308,6 +2308,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="O6:O15"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
@@ -2324,30 +2348,6 @@
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O6:O15"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2376,20 +2376,20 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51" t="s">
+      <c r="G2" s="68"/>
+      <c r="H2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="70"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2398,23 +2398,23 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="57">
+      <c r="C3" s="73">
         <v>1</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="74"/>
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="55" t="s">
+      <c r="G3" s="72"/>
+      <c r="H3" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2423,22 +2423,22 @@
       <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47" t="s">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
       <c r="L5" s="16" t="s">
         <v>7</v>
       </c>
@@ -2450,41 +2450,41 @@
       <c r="A6" s="22">
         <v>1</v>
       </c>
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="105"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="80"/>
     </row>
     <row r="7" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="88" t="s">
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="97" t="s">
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="99"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="95"/>
       <c r="L7" s="20" t="s">
         <v>18</v>
       </c>
@@ -2494,22 +2494,22 @@
       <c r="A8" s="24">
         <v>1.2</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="112" t="s">
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="113"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="97" t="s">
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="99"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="95"/>
       <c r="L8" s="18" t="s">
         <v>18</v>
       </c>
@@ -2519,22 +2519,22 @@
       <c r="A9" s="25">
         <v>1.3</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="92" t="s">
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="97" t="s">
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="99"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="95"/>
       <c r="L9" s="19" t="s">
         <v>18</v>
       </c>
@@ -2544,41 +2544,41 @@
       <c r="A10" s="22">
         <v>2</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="105"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="80"/>
     </row>
     <row r="11" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23">
         <v>2.1</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="88" t="s">
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="97" t="s">
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="99"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="95"/>
       <c r="L11" s="20" t="s">
         <v>19</v>
       </c>
@@ -2588,22 +2588,22 @@
       <c r="A12" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="90" t="s">
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="91"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="77" t="s">
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="79"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="110"/>
       <c r="L12" s="18" t="s">
         <v>19</v>
       </c>
@@ -2615,22 +2615,22 @@
       <c r="A13" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="92" t="s">
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="94" t="s">
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="96"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="113"/>
       <c r="L13" s="19" t="s">
         <v>19</v>
       </c>
@@ -2640,41 +2640,41 @@
       <c r="A14" s="22">
         <v>3</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
-      <c r="M14" s="105"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="80"/>
     </row>
     <row r="15" spans="1:14" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23">
         <v>3.1</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="100" t="s">
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="97" t="s">
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="99"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="95"/>
       <c r="L15" s="20" t="s">
         <v>19</v>
       </c>
@@ -2684,22 +2684,22 @@
       <c r="A16" s="24">
         <v>3.2</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="90" t="s">
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="77" t="s">
+      <c r="F16" s="107"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="79"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="109"/>
+      <c r="K16" s="110"/>
       <c r="L16" s="18" t="s">
         <v>19</v>
       </c>
@@ -2711,22 +2711,22 @@
       <c r="A17" s="25">
         <v>3.3</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="92" t="s">
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="94" t="s">
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="96"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="113"/>
       <c r="L17" s="19" t="s">
         <v>19</v>
       </c>
@@ -2736,41 +2736,41 @@
       <c r="A18" s="22">
         <v>4</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="104"/>
-      <c r="J18" s="104"/>
-      <c r="K18" s="104"/>
-      <c r="L18" s="104"/>
-      <c r="M18" s="105"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="80"/>
     </row>
     <row r="19" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="26">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B19" s="103" t="s">
+      <c r="B19" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76" t="s">
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="80" t="s">
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
       <c r="L19" s="27" t="s">
         <v>19</v>
       </c>
@@ -2782,22 +2782,22 @@
       <c r="A20" s="26">
         <v>4.3</v>
       </c>
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="106" t="s">
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="107"/>
-      <c r="G20" s="108"/>
-      <c r="H20" s="109" t="s">
+      <c r="F20" s="84"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="110"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="111"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="88"/>
       <c r="L20" s="27" t="s">
         <v>19</v>
       </c>
@@ -2809,22 +2809,22 @@
       <c r="A21" s="26">
         <v>4.2</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76" t="s">
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="80" t="s">
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
       <c r="L21" s="27" t="s">
         <v>19</v>
       </c>
@@ -2854,6 +2854,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:K5"/>
@@ -2870,39 +2903,6 @@
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:G8"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2913,7 +2913,7 @@
   <dimension ref="A1:N80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:K8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2929,20 +2929,20 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="F2" s="49" t="s">
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51" t="s">
+      <c r="G2" s="68"/>
+      <c r="H2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="70"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2951,23 +2951,23 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="57">
+      <c r="C3" s="73">
         <v>1</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="74"/>
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="55" t="s">
+      <c r="G3" s="72"/>
+      <c r="H3" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2975,22 +2975,22 @@
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60" t="s">
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
       <c r="L5" s="32" t="s">
         <v>7</v>
       </c>
@@ -3002,41 +3002,41 @@
       <c r="A6" s="36">
         <v>1</v>
       </c>
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="132" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="114"/>
-      <c r="M6" s="114"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="127" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="115"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115" t="s">
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127" t="s">
         <v>180</v>
       </c>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115" t="s">
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="127" t="s">
         <v>180</v>
       </c>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
       <c r="L7" s="35" t="s">
         <v>19</v>
       </c>
@@ -3046,81 +3046,85 @@
       <c r="A8" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="127" t="s">
         <v>179</v>
       </c>
-      <c r="C8" s="115"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115" t="s">
+      <c r="C8" s="127"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127" t="s">
         <v>181</v>
       </c>
-      <c r="F8" s="115"/>
-      <c r="G8" s="115"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="115"/>
-      <c r="L8" s="35"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="127"/>
+      <c r="H8" s="127" t="s">
+        <v>181</v>
+      </c>
+      <c r="I8" s="127"/>
+      <c r="J8" s="127"/>
+      <c r="K8" s="127"/>
+      <c r="L8" s="35" t="s">
+        <v>19</v>
+      </c>
       <c r="M8" s="35"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36">
         <v>2</v>
       </c>
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="132" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
+      <c r="K9" s="132"/>
+      <c r="L9" s="132"/>
+      <c r="M9" s="132"/>
     </row>
     <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>2.1</v>
       </c>
-      <c r="B10" s="115" t="s">
+      <c r="B10" s="127" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
-      <c r="G10" s="115"/>
-      <c r="H10" s="115"/>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="115"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="127"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="127"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="127" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115" t="s">
+      <c r="C11" s="127"/>
+      <c r="D11" s="127"/>
+      <c r="E11" s="127" t="s">
         <v>126</v>
       </c>
-      <c r="F11" s="115"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="116" t="s">
+      <c r="F11" s="127"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="117" t="s">
         <v>126</v>
       </c>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="119"/>
       <c r="L11" s="34" t="s">
         <v>19</v>
       </c>
@@ -3130,22 +3134,22 @@
       <c r="A12" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="115" t="s">
+      <c r="B12" s="127" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="115"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115" t="s">
+      <c r="C12" s="127"/>
+      <c r="D12" s="127"/>
+      <c r="E12" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="115"/>
-      <c r="G12" s="115"/>
-      <c r="H12" s="116" t="s">
+      <c r="F12" s="127"/>
+      <c r="G12" s="127"/>
+      <c r="H12" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="I12" s="117"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="119"/>
       <c r="L12" s="34" t="s">
         <v>19</v>
       </c>
@@ -3157,41 +3161,41 @@
       <c r="A13" s="18">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B13" s="115" t="s">
+      <c r="B13" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="115"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="115"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
+      <c r="C13" s="127"/>
+      <c r="D13" s="127"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="127"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
+      <c r="K13" s="127"/>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
     </row>
     <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="127" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="115"/>
-      <c r="D14" s="115"/>
-      <c r="E14" s="115" t="s">
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="127" t="s">
         <v>127</v>
       </c>
-      <c r="F14" s="115"/>
-      <c r="G14" s="115"/>
-      <c r="H14" s="116" t="s">
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="117" t="s">
         <v>127</v>
       </c>
-      <c r="I14" s="117"/>
-      <c r="J14" s="117"/>
-      <c r="K14" s="118"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="118"/>
+      <c r="K14" s="119"/>
       <c r="L14" s="34" t="s">
         <v>19</v>
       </c>
@@ -3201,22 +3205,22 @@
       <c r="A15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="115" t="s">
+      <c r="B15" s="127" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="115"/>
-      <c r="E15" s="115" t="s">
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="115"/>
-      <c r="G15" s="115"/>
-      <c r="H15" s="116" t="s">
+      <c r="F15" s="127"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="117"/>
-      <c r="J15" s="117"/>
-      <c r="K15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="119"/>
       <c r="L15" s="34" t="s">
         <v>19</v>
       </c>
@@ -3228,41 +3232,41 @@
       <c r="A16" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="127" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="115"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="115"/>
-      <c r="G16" s="115"/>
-      <c r="H16" s="115"/>
-      <c r="I16" s="115"/>
-      <c r="J16" s="115"/>
-      <c r="K16" s="115"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="115"/>
+      <c r="C16" s="127"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
     </row>
     <row r="17" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="115" t="s">
+      <c r="B17" s="127" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115" t="s">
+      <c r="C17" s="127"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="127" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="116" t="s">
+      <c r="F17" s="127"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="117" t="s">
         <v>115</v>
       </c>
-      <c r="I17" s="117"/>
-      <c r="J17" s="117"/>
-      <c r="K17" s="118"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="119"/>
       <c r="L17" s="33" t="s">
         <v>19</v>
       </c>
@@ -3272,22 +3276,22 @@
       <c r="A18" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="127" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="115"/>
-      <c r="D18" s="115"/>
-      <c r="E18" s="115" t="s">
+      <c r="C18" s="127"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="115"/>
-      <c r="G18" s="115"/>
-      <c r="H18" s="116" t="s">
+      <c r="F18" s="127"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="I18" s="117"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="119"/>
       <c r="L18" s="34" t="s">
         <v>19</v>
       </c>
@@ -3299,22 +3303,22 @@
       <c r="A19" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="127" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115" t="s">
+      <c r="C19" s="127"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
-      <c r="H19" s="116" t="s">
+      <c r="F19" s="127"/>
+      <c r="G19" s="127"/>
+      <c r="H19" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="I19" s="117"/>
-      <c r="J19" s="117"/>
-      <c r="K19" s="118"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="119"/>
       <c r="L19" s="34" t="s">
         <v>19</v>
       </c>
@@ -3326,41 +3330,41 @@
       <c r="A20" s="18">
         <v>2.4</v>
       </c>
-      <c r="B20" s="115" t="s">
+      <c r="B20" s="127" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="115"/>
-      <c r="H20" s="115"/>
-      <c r="I20" s="115"/>
-      <c r="J20" s="115"/>
-      <c r="K20" s="115"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="127"/>
+      <c r="K20" s="127"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="127"/>
     </row>
     <row r="21" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="115" t="s">
+      <c r="B21" s="127" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="115"/>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115" t="s">
+      <c r="C21" s="127"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="115"/>
-      <c r="G21" s="115"/>
-      <c r="H21" s="116" t="s">
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="117"/>
-      <c r="J21" s="117"/>
-      <c r="K21" s="118"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="119"/>
       <c r="L21" s="34" t="s">
         <v>19</v>
       </c>
@@ -3370,22 +3374,22 @@
       <c r="A22" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="116" t="s">
+      <c r="B22" s="117" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="117"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="115" t="s">
+      <c r="C22" s="118"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="115"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="116" t="s">
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="117" t="s">
         <v>118</v>
       </c>
-      <c r="I22" s="117"/>
-      <c r="J22" s="117"/>
-      <c r="K22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="119"/>
       <c r="L22" s="34" t="s">
         <v>19</v>
       </c>
@@ -3397,22 +3401,22 @@
       <c r="A23" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="116" t="s">
+      <c r="B23" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="117"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="115" t="s">
+      <c r="C23" s="118"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="115"/>
-      <c r="G23" s="115"/>
-      <c r="H23" s="116" t="s">
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="117" t="s">
         <v>117</v>
       </c>
-      <c r="I23" s="117"/>
-      <c r="J23" s="117"/>
-      <c r="K23" s="118"/>
+      <c r="I23" s="118"/>
+      <c r="J23" s="118"/>
+      <c r="K23" s="119"/>
       <c r="L23" s="34" t="s">
         <v>19</v>
       </c>
@@ -3424,41 +3428,41 @@
       <c r="A24" s="18">
         <v>2.5</v>
       </c>
-      <c r="B24" s="116" t="s">
+      <c r="B24" s="117" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="117"/>
-      <c r="D24" s="117"/>
-      <c r="E24" s="117"/>
-      <c r="F24" s="117"/>
-      <c r="G24" s="117"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="117"/>
-      <c r="L24" s="117"/>
-      <c r="M24" s="118"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
+      <c r="G24" s="118"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="118"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="118"/>
+      <c r="L24" s="118"/>
+      <c r="M24" s="119"/>
     </row>
     <row r="25" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="115" t="s">
+      <c r="B25" s="127" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="115"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="115" t="s">
+      <c r="C25" s="127"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127" t="s">
         <v>143</v>
       </c>
-      <c r="F25" s="115"/>
-      <c r="G25" s="115"/>
-      <c r="H25" s="116" t="s">
+      <c r="F25" s="127"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="117" t="s">
         <v>143</v>
       </c>
-      <c r="I25" s="117"/>
-      <c r="J25" s="117"/>
-      <c r="K25" s="118"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="118"/>
+      <c r="K25" s="119"/>
       <c r="L25" s="34" t="s">
         <v>19</v>
       </c>
@@ -3468,22 +3472,22 @@
       <c r="A26" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="116" t="s">
+      <c r="B26" s="117" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="117"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="115" t="s">
+      <c r="C26" s="118"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
-      <c r="H26" s="116" t="s">
+      <c r="F26" s="127"/>
+      <c r="G26" s="127"/>
+      <c r="H26" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="I26" s="117"/>
-      <c r="J26" s="117"/>
-      <c r="K26" s="118"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="119"/>
       <c r="L26" s="34" t="s">
         <v>19</v>
       </c>
@@ -3495,22 +3499,22 @@
       <c r="A27" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="116" t="s">
+      <c r="B27" s="117" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="117"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="115" t="s">
+      <c r="C27" s="118"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="116" t="s">
+      <c r="F27" s="127"/>
+      <c r="G27" s="127"/>
+      <c r="H27" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="I27" s="117"/>
-      <c r="J27" s="117"/>
-      <c r="K27" s="118"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="119"/>
       <c r="L27" s="34" t="s">
         <v>19</v>
       </c>
@@ -3522,41 +3526,41 @@
       <c r="A28" s="18">
         <v>2.6</v>
       </c>
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="127" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="115"/>
-      <c r="D28" s="115"/>
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="115"/>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="115"/>
-      <c r="L28" s="115"/>
-      <c r="M28" s="115"/>
+      <c r="C28" s="127"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="127"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="127"/>
+      <c r="J28" s="127"/>
+      <c r="K28" s="127"/>
+      <c r="L28" s="127"/>
+      <c r="M28" s="127"/>
     </row>
     <row r="29" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="115" t="s">
+      <c r="B29" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="115"/>
-      <c r="D29" s="115"/>
-      <c r="E29" s="115" t="s">
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="127" t="s">
         <v>144</v>
       </c>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="116" t="s">
+      <c r="F29" s="127"/>
+      <c r="G29" s="127"/>
+      <c r="H29" s="117" t="s">
         <v>144</v>
       </c>
-      <c r="I29" s="117"/>
-      <c r="J29" s="117"/>
-      <c r="K29" s="118"/>
+      <c r="I29" s="118"/>
+      <c r="J29" s="118"/>
+      <c r="K29" s="119"/>
       <c r="L29" s="34" t="s">
         <v>19</v>
       </c>
@@ -3566,22 +3570,22 @@
       <c r="A30" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="115" t="s">
+      <c r="B30" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="115"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115" t="s">
+      <c r="C30" s="127"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
-      <c r="H30" s="116" t="s">
+      <c r="F30" s="127"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="I30" s="117"/>
-      <c r="J30" s="117"/>
-      <c r="K30" s="118"/>
+      <c r="I30" s="118"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="119"/>
       <c r="L30" s="34" t="s">
         <v>19</v>
       </c>
@@ -3593,41 +3597,41 @@
       <c r="A31" s="18">
         <v>2.7</v>
       </c>
-      <c r="B31" s="115" t="s">
+      <c r="B31" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="115"/>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="115"/>
-      <c r="I31" s="115"/>
-      <c r="J31" s="115"/>
-      <c r="K31" s="115"/>
-      <c r="L31" s="115"/>
-      <c r="M31" s="115"/>
+      <c r="C31" s="127"/>
+      <c r="D31" s="127"/>
+      <c r="E31" s="127"/>
+      <c r="F31" s="127"/>
+      <c r="G31" s="127"/>
+      <c r="H31" s="127"/>
+      <c r="I31" s="127"/>
+      <c r="J31" s="127"/>
+      <c r="K31" s="127"/>
+      <c r="L31" s="127"/>
+      <c r="M31" s="127"/>
     </row>
     <row r="32" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="115" t="s">
+      <c r="B32" s="127" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="115"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115" t="s">
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="127" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
-      <c r="H32" s="116" t="s">
+      <c r="F32" s="127"/>
+      <c r="G32" s="127"/>
+      <c r="H32" s="117" t="s">
         <v>145</v>
       </c>
-      <c r="I32" s="117"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="118"/>
+      <c r="I32" s="118"/>
+      <c r="J32" s="118"/>
+      <c r="K32" s="119"/>
       <c r="L32" s="34" t="s">
         <v>19</v>
       </c>
@@ -3637,22 +3641,22 @@
       <c r="A33" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="115" t="s">
+      <c r="B33" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="115"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="115" t="s">
+      <c r="C33" s="127"/>
+      <c r="D33" s="127"/>
+      <c r="E33" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="115"/>
-      <c r="G33" s="115"/>
-      <c r="H33" s="116" t="s">
+      <c r="F33" s="127"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="117" t="s">
         <v>129</v>
       </c>
-      <c r="I33" s="117"/>
-      <c r="J33" s="117"/>
-      <c r="K33" s="118"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="118"/>
+      <c r="K33" s="119"/>
       <c r="L33" s="34" t="s">
         <v>19</v>
       </c>
@@ -3662,41 +3666,41 @@
       <c r="A34" s="37">
         <v>2.8</v>
       </c>
-      <c r="B34" s="119" t="s">
+      <c r="B34" s="133" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="119"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="119"/>
-      <c r="F34" s="119"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="119"/>
-      <c r="I34" s="119"/>
-      <c r="J34" s="119"/>
-      <c r="K34" s="119"/>
-      <c r="L34" s="119"/>
-      <c r="M34" s="119"/>
+      <c r="C34" s="133"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="133"/>
+      <c r="G34" s="133"/>
+      <c r="H34" s="133"/>
+      <c r="I34" s="133"/>
+      <c r="J34" s="133"/>
+      <c r="K34" s="133"/>
+      <c r="L34" s="133"/>
+      <c r="M34" s="133"/>
     </row>
     <row r="35" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="123" t="s">
+      <c r="B35" s="128" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="123"/>
-      <c r="D35" s="123"/>
-      <c r="E35" s="123" t="s">
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="128" t="s">
         <v>146</v>
       </c>
-      <c r="F35" s="123"/>
-      <c r="G35" s="123"/>
-      <c r="H35" s="120" t="s">
+      <c r="F35" s="128"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="129" t="s">
         <v>150</v>
       </c>
-      <c r="I35" s="121"/>
-      <c r="J35" s="121"/>
-      <c r="K35" s="122"/>
+      <c r="I35" s="130"/>
+      <c r="J35" s="130"/>
+      <c r="K35" s="131"/>
       <c r="L35" s="34" t="s">
         <v>19</v>
       </c>
@@ -3708,22 +3712,22 @@
       <c r="A36" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="123" t="s">
+      <c r="B36" s="128" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="123"/>
-      <c r="D36" s="123"/>
-      <c r="E36" s="123" t="s">
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
+      <c r="E36" s="128" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="123"/>
-      <c r="G36" s="123"/>
-      <c r="H36" s="120" t="s">
+      <c r="F36" s="128"/>
+      <c r="G36" s="128"/>
+      <c r="H36" s="129" t="s">
         <v>151</v>
       </c>
-      <c r="I36" s="121"/>
-      <c r="J36" s="121"/>
-      <c r="K36" s="122"/>
+      <c r="I36" s="130"/>
+      <c r="J36" s="130"/>
+      <c r="K36" s="131"/>
       <c r="L36" s="34" t="s">
         <v>19</v>
       </c>
@@ -3735,22 +3739,22 @@
       <c r="A37" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="123" t="s">
+      <c r="B37" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="123"/>
-      <c r="D37" s="123"/>
-      <c r="E37" s="123" t="s">
+      <c r="C37" s="128"/>
+      <c r="D37" s="128"/>
+      <c r="E37" s="128" t="s">
         <v>147</v>
       </c>
-      <c r="F37" s="123"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="120" t="s">
+      <c r="F37" s="128"/>
+      <c r="G37" s="128"/>
+      <c r="H37" s="129" t="s">
         <v>152</v>
       </c>
-      <c r="I37" s="121"/>
-      <c r="J37" s="121"/>
-      <c r="K37" s="122"/>
+      <c r="I37" s="130"/>
+      <c r="J37" s="130"/>
+      <c r="K37" s="131"/>
       <c r="L37" s="34" t="s">
         <v>19</v>
       </c>
@@ -3762,41 +3766,41 @@
       <c r="A38" s="18">
         <v>2.9</v>
       </c>
-      <c r="B38" s="115" t="s">
+      <c r="B38" s="127" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="115"/>
-      <c r="D38" s="115"/>
-      <c r="E38" s="115"/>
-      <c r="F38" s="115"/>
-      <c r="G38" s="115"/>
-      <c r="H38" s="115"/>
-      <c r="I38" s="115"/>
-      <c r="J38" s="115"/>
-      <c r="K38" s="115"/>
-      <c r="L38" s="115"/>
-      <c r="M38" s="115"/>
+      <c r="C38" s="127"/>
+      <c r="D38" s="127"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="127"/>
+      <c r="G38" s="127"/>
+      <c r="H38" s="127"/>
+      <c r="I38" s="127"/>
+      <c r="J38" s="127"/>
+      <c r="K38" s="127"/>
+      <c r="L38" s="127"/>
+      <c r="M38" s="127"/>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="115" t="s">
+      <c r="B39" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="115"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="116" t="s">
+      <c r="C39" s="127"/>
+      <c r="D39" s="127"/>
+      <c r="E39" s="117" t="s">
         <v>126</v>
       </c>
-      <c r="F39" s="117"/>
-      <c r="G39" s="118"/>
-      <c r="H39" s="116" t="s">
+      <c r="F39" s="118"/>
+      <c r="G39" s="119"/>
+      <c r="H39" s="117" t="s">
         <v>153</v>
       </c>
-      <c r="I39" s="117"/>
-      <c r="J39" s="117"/>
-      <c r="K39" s="118"/>
+      <c r="I39" s="118"/>
+      <c r="J39" s="118"/>
+      <c r="K39" s="119"/>
       <c r="L39" s="34" t="s">
         <v>19</v>
       </c>
@@ -3806,22 +3810,22 @@
       <c r="A40" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="115" t="s">
+      <c r="B40" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="115"/>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115" t="s">
+      <c r="C40" s="127"/>
+      <c r="D40" s="127"/>
+      <c r="E40" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="F40" s="115"/>
-      <c r="G40" s="115"/>
-      <c r="H40" s="116" t="s">
+      <c r="F40" s="127"/>
+      <c r="G40" s="127"/>
+      <c r="H40" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="I40" s="117"/>
-      <c r="J40" s="117"/>
-      <c r="K40" s="118"/>
+      <c r="I40" s="118"/>
+      <c r="J40" s="118"/>
+      <c r="K40" s="119"/>
       <c r="L40" s="34" t="s">
         <v>19</v>
       </c>
@@ -3831,22 +3835,22 @@
       <c r="A41" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="115" t="s">
+      <c r="B41" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="115"/>
-      <c r="D41" s="115"/>
-      <c r="E41" s="116" t="s">
+      <c r="C41" s="127"/>
+      <c r="D41" s="127"/>
+      <c r="E41" s="117" t="s">
         <v>144</v>
       </c>
-      <c r="F41" s="117"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="116" t="s">
+      <c r="F41" s="118"/>
+      <c r="G41" s="119"/>
+      <c r="H41" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="I41" s="117"/>
-      <c r="J41" s="117"/>
-      <c r="K41" s="118"/>
+      <c r="I41" s="118"/>
+      <c r="J41" s="118"/>
+      <c r="K41" s="119"/>
       <c r="L41" s="34" t="s">
         <v>19</v>
       </c>
@@ -3856,41 +3860,41 @@
       <c r="A42" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="115" t="s">
+      <c r="B42" s="127" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="115"/>
-      <c r="D42" s="115"/>
-      <c r="E42" s="115"/>
-      <c r="F42" s="115"/>
-      <c r="G42" s="115"/>
-      <c r="H42" s="115"/>
-      <c r="I42" s="115"/>
-      <c r="J42" s="115"/>
-      <c r="K42" s="115"/>
-      <c r="L42" s="115"/>
-      <c r="M42" s="115"/>
+      <c r="C42" s="127"/>
+      <c r="D42" s="127"/>
+      <c r="E42" s="127"/>
+      <c r="F42" s="127"/>
+      <c r="G42" s="127"/>
+      <c r="H42" s="127"/>
+      <c r="I42" s="127"/>
+      <c r="J42" s="127"/>
+      <c r="K42" s="127"/>
+      <c r="L42" s="127"/>
+      <c r="M42" s="127"/>
     </row>
     <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="115" t="s">
+      <c r="B43" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="115"/>
-      <c r="D43" s="115"/>
-      <c r="E43" s="115" t="s">
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
+      <c r="E43" s="127" t="s">
         <v>127</v>
       </c>
-      <c r="F43" s="115"/>
-      <c r="G43" s="115"/>
-      <c r="H43" s="116" t="s">
+      <c r="F43" s="127"/>
+      <c r="G43" s="127"/>
+      <c r="H43" s="117" t="s">
         <v>156</v>
       </c>
-      <c r="I43" s="117"/>
-      <c r="J43" s="117"/>
-      <c r="K43" s="118"/>
+      <c r="I43" s="118"/>
+      <c r="J43" s="118"/>
+      <c r="K43" s="119"/>
       <c r="L43" s="34" t="s">
         <v>19</v>
       </c>
@@ -3900,22 +3904,22 @@
       <c r="A44" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="115" t="s">
+      <c r="B44" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="115"/>
-      <c r="D44" s="115"/>
-      <c r="E44" s="115" t="s">
+      <c r="C44" s="127"/>
+      <c r="D44" s="127"/>
+      <c r="E44" s="127" t="s">
         <v>148</v>
       </c>
-      <c r="F44" s="115"/>
-      <c r="G44" s="115"/>
-      <c r="H44" s="116" t="s">
+      <c r="F44" s="127"/>
+      <c r="G44" s="127"/>
+      <c r="H44" s="117" t="s">
         <v>157</v>
       </c>
-      <c r="I44" s="117"/>
-      <c r="J44" s="117"/>
-      <c r="K44" s="118"/>
+      <c r="I44" s="118"/>
+      <c r="J44" s="118"/>
+      <c r="K44" s="119"/>
       <c r="L44" s="34" t="s">
         <v>19</v>
       </c>
@@ -3925,22 +3929,22 @@
       <c r="A45" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="115" t="s">
+      <c r="B45" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="115"/>
-      <c r="D45" s="115"/>
-      <c r="E45" s="115" t="s">
+      <c r="C45" s="127"/>
+      <c r="D45" s="127"/>
+      <c r="E45" s="127" t="s">
         <v>149</v>
       </c>
-      <c r="F45" s="115"/>
-      <c r="G45" s="115"/>
-      <c r="H45" s="116" t="s">
+      <c r="F45" s="127"/>
+      <c r="G45" s="127"/>
+      <c r="H45" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="I45" s="117"/>
-      <c r="J45" s="117"/>
-      <c r="K45" s="118"/>
+      <c r="I45" s="118"/>
+      <c r="J45" s="118"/>
+      <c r="K45" s="119"/>
       <c r="L45" s="34" t="s">
         <v>19</v>
       </c>
@@ -3950,41 +3954,41 @@
       <c r="A46" s="18">
         <v>2.11</v>
       </c>
-      <c r="B46" s="115" t="s">
+      <c r="B46" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="C46" s="115"/>
-      <c r="D46" s="115"/>
-      <c r="E46" s="115"/>
-      <c r="F46" s="115"/>
-      <c r="G46" s="115"/>
-      <c r="H46" s="115"/>
-      <c r="I46" s="115"/>
-      <c r="J46" s="115"/>
-      <c r="K46" s="115"/>
-      <c r="L46" s="115"/>
-      <c r="M46" s="115"/>
+      <c r="C46" s="127"/>
+      <c r="D46" s="127"/>
+      <c r="E46" s="127"/>
+      <c r="F46" s="127"/>
+      <c r="G46" s="127"/>
+      <c r="H46" s="127"/>
+      <c r="I46" s="127"/>
+      <c r="J46" s="127"/>
+      <c r="K46" s="127"/>
+      <c r="L46" s="127"/>
+      <c r="M46" s="127"/>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="115" t="s">
+      <c r="B47" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="C47" s="115"/>
-      <c r="D47" s="115"/>
-      <c r="E47" s="116" t="s">
+      <c r="C47" s="127"/>
+      <c r="D47" s="127"/>
+      <c r="E47" s="117" t="s">
         <v>126</v>
       </c>
-      <c r="F47" s="117"/>
-      <c r="G47" s="118"/>
-      <c r="H47" s="116" t="s">
+      <c r="F47" s="118"/>
+      <c r="G47" s="119"/>
+      <c r="H47" s="117" t="s">
         <v>163</v>
       </c>
-      <c r="I47" s="117"/>
-      <c r="J47" s="117"/>
-      <c r="K47" s="118"/>
+      <c r="I47" s="118"/>
+      <c r="J47" s="118"/>
+      <c r="K47" s="119"/>
       <c r="L47" s="38" t="s">
         <v>19</v>
       </c>
@@ -3996,22 +4000,22 @@
       <c r="A48" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B48" s="115" t="s">
+      <c r="B48" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="C48" s="115"/>
-      <c r="D48" s="115"/>
-      <c r="E48" s="115" t="s">
+      <c r="C48" s="127"/>
+      <c r="D48" s="127"/>
+      <c r="E48" s="127" t="s">
         <v>148</v>
       </c>
-      <c r="F48" s="115"/>
-      <c r="G48" s="115"/>
-      <c r="H48" s="116" t="s">
+      <c r="F48" s="127"/>
+      <c r="G48" s="127"/>
+      <c r="H48" s="117" t="s">
         <v>157</v>
       </c>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="118"/>
+      <c r="I48" s="118"/>
+      <c r="J48" s="118"/>
+      <c r="K48" s="119"/>
       <c r="L48" s="38" t="s">
         <v>19</v>
       </c>
@@ -4023,22 +4027,22 @@
       <c r="A49" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="115" t="s">
+      <c r="B49" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="C49" s="115"/>
-      <c r="D49" s="115"/>
-      <c r="E49" s="116" t="s">
+      <c r="C49" s="127"/>
+      <c r="D49" s="127"/>
+      <c r="E49" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="F49" s="117"/>
-      <c r="G49" s="118"/>
-      <c r="H49" s="116" t="s">
+      <c r="F49" s="118"/>
+      <c r="G49" s="119"/>
+      <c r="H49" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="I49" s="117"/>
-      <c r="J49" s="117"/>
-      <c r="K49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="119"/>
       <c r="L49" s="38" t="s">
         <v>19</v>
       </c>
@@ -4050,41 +4054,41 @@
       <c r="A50" s="18">
         <v>2.12</v>
       </c>
-      <c r="B50" s="116" t="s">
+      <c r="B50" s="117" t="s">
         <v>160</v>
       </c>
-      <c r="C50" s="117"/>
-      <c r="D50" s="117"/>
-      <c r="E50" s="117"/>
-      <c r="F50" s="117"/>
-      <c r="G50" s="117"/>
-      <c r="H50" s="117"/>
-      <c r="I50" s="117"/>
-      <c r="J50" s="117"/>
-      <c r="K50" s="117"/>
-      <c r="L50" s="117"/>
-      <c r="M50" s="118"/>
+      <c r="C50" s="118"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="118"/>
+      <c r="F50" s="118"/>
+      <c r="G50" s="118"/>
+      <c r="H50" s="118"/>
+      <c r="I50" s="118"/>
+      <c r="J50" s="118"/>
+      <c r="K50" s="118"/>
+      <c r="L50" s="118"/>
+      <c r="M50" s="119"/>
     </row>
     <row r="51" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="B51" s="115" t="s">
+      <c r="B51" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="115"/>
-      <c r="D51" s="115"/>
-      <c r="E51" s="116" t="s">
+      <c r="C51" s="127"/>
+      <c r="D51" s="127"/>
+      <c r="E51" s="117" t="s">
         <v>127</v>
       </c>
-      <c r="F51" s="117"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="116" t="s">
+      <c r="F51" s="118"/>
+      <c r="G51" s="119"/>
+      <c r="H51" s="117" t="s">
         <v>156</v>
       </c>
-      <c r="I51" s="117"/>
-      <c r="J51" s="117"/>
-      <c r="K51" s="118"/>
+      <c r="I51" s="118"/>
+      <c r="J51" s="118"/>
+      <c r="K51" s="119"/>
       <c r="L51" s="38" t="s">
         <v>19</v>
       </c>
@@ -4096,22 +4100,22 @@
       <c r="A52" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B52" s="115" t="s">
+      <c r="B52" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="115"/>
-      <c r="D52" s="115"/>
-      <c r="E52" s="115" t="s">
+      <c r="C52" s="127"/>
+      <c r="D52" s="127"/>
+      <c r="E52" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="F52" s="115"/>
-      <c r="G52" s="115"/>
-      <c r="H52" s="116" t="s">
+      <c r="F52" s="127"/>
+      <c r="G52" s="127"/>
+      <c r="H52" s="117" t="s">
         <v>165</v>
       </c>
-      <c r="I52" s="117"/>
-      <c r="J52" s="117"/>
-      <c r="K52" s="118"/>
+      <c r="I52" s="118"/>
+      <c r="J52" s="118"/>
+      <c r="K52" s="119"/>
       <c r="L52" s="38" t="s">
         <v>19</v>
       </c>
@@ -4123,22 +4127,22 @@
       <c r="A53" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B53" s="115" t="s">
+      <c r="B53" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="115"/>
-      <c r="D53" s="115"/>
-      <c r="E53" s="116" t="s">
+      <c r="C53" s="127"/>
+      <c r="D53" s="127"/>
+      <c r="E53" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="F53" s="117"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="116" t="s">
+      <c r="F53" s="118"/>
+      <c r="G53" s="119"/>
+      <c r="H53" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="I53" s="117"/>
-      <c r="J53" s="117"/>
-      <c r="K53" s="118"/>
+      <c r="I53" s="118"/>
+      <c r="J53" s="118"/>
+      <c r="K53" s="119"/>
       <c r="L53" s="38" t="s">
         <v>19</v>
       </c>
@@ -4150,41 +4154,41 @@
       <c r="A54" s="18">
         <v>2.13</v>
       </c>
-      <c r="B54" s="115" t="s">
+      <c r="B54" s="127" t="s">
         <v>161</v>
       </c>
-      <c r="C54" s="115"/>
-      <c r="D54" s="115"/>
-      <c r="E54" s="115"/>
-      <c r="F54" s="115"/>
-      <c r="G54" s="115"/>
-      <c r="H54" s="115"/>
-      <c r="I54" s="115"/>
-      <c r="J54" s="115"/>
-      <c r="K54" s="115"/>
-      <c r="L54" s="115"/>
-      <c r="M54" s="115"/>
+      <c r="C54" s="127"/>
+      <c r="D54" s="127"/>
+      <c r="E54" s="127"/>
+      <c r="F54" s="127"/>
+      <c r="G54" s="127"/>
+      <c r="H54" s="127"/>
+      <c r="I54" s="127"/>
+      <c r="J54" s="127"/>
+      <c r="K54" s="127"/>
+      <c r="L54" s="127"/>
+      <c r="M54" s="127"/>
     </row>
     <row r="55" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="B55" s="115" t="s">
+      <c r="B55" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="115"/>
-      <c r="D55" s="115"/>
-      <c r="E55" s="116" t="s">
+      <c r="C55" s="127"/>
+      <c r="D55" s="127"/>
+      <c r="E55" s="117" t="s">
         <v>127</v>
       </c>
-      <c r="F55" s="117"/>
-      <c r="G55" s="118"/>
-      <c r="H55" s="116" t="s">
+      <c r="F55" s="118"/>
+      <c r="G55" s="119"/>
+      <c r="H55" s="117" t="s">
         <v>156</v>
       </c>
-      <c r="I55" s="117"/>
-      <c r="J55" s="117"/>
-      <c r="K55" s="118"/>
+      <c r="I55" s="118"/>
+      <c r="J55" s="118"/>
+      <c r="K55" s="119"/>
       <c r="L55" s="38" t="s">
         <v>19</v>
       </c>
@@ -4196,22 +4200,22 @@
       <c r="A56" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="B56" s="115" t="s">
+      <c r="B56" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="115"/>
-      <c r="D56" s="115"/>
-      <c r="E56" s="115" t="s">
+      <c r="C56" s="127"/>
+      <c r="D56" s="127"/>
+      <c r="E56" s="127" t="s">
         <v>148</v>
       </c>
-      <c r="F56" s="115"/>
-      <c r="G56" s="115"/>
-      <c r="H56" s="116" t="s">
+      <c r="F56" s="127"/>
+      <c r="G56" s="127"/>
+      <c r="H56" s="117" t="s">
         <v>157</v>
       </c>
-      <c r="I56" s="117"/>
-      <c r="J56" s="117"/>
-      <c r="K56" s="118"/>
+      <c r="I56" s="118"/>
+      <c r="J56" s="118"/>
+      <c r="K56" s="119"/>
       <c r="L56" s="38" t="s">
         <v>19</v>
       </c>
@@ -4223,22 +4227,22 @@
       <c r="A57" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="B57" s="115" t="s">
+      <c r="B57" s="127" t="s">
         <v>128</v>
       </c>
-      <c r="C57" s="115"/>
-      <c r="D57" s="115"/>
-      <c r="E57" s="116" t="s">
+      <c r="C57" s="127"/>
+      <c r="D57" s="127"/>
+      <c r="E57" s="117" t="s">
         <v>144</v>
       </c>
-      <c r="F57" s="117"/>
-      <c r="G57" s="118"/>
-      <c r="H57" s="116" t="s">
+      <c r="F57" s="118"/>
+      <c r="G57" s="119"/>
+      <c r="H57" s="117" t="s">
         <v>166</v>
       </c>
-      <c r="I57" s="117"/>
-      <c r="J57" s="117"/>
-      <c r="K57" s="118"/>
+      <c r="I57" s="118"/>
+      <c r="J57" s="118"/>
+      <c r="K57" s="119"/>
       <c r="L57" s="38" t="s">
         <v>19</v>
       </c>
@@ -4250,58 +4254,58 @@
       <c r="A58" s="36">
         <v>3</v>
       </c>
-      <c r="B58" s="114" t="s">
+      <c r="B58" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="114"/>
-      <c r="D58" s="114"/>
-      <c r="E58" s="114"/>
-      <c r="F58" s="114"/>
-      <c r="G58" s="114"/>
-      <c r="H58" s="114"/>
-      <c r="I58" s="114"/>
-      <c r="J58" s="114"/>
-      <c r="K58" s="114"/>
-      <c r="L58" s="114"/>
-      <c r="M58" s="114"/>
+      <c r="C58" s="132"/>
+      <c r="D58" s="132"/>
+      <c r="E58" s="132"/>
+      <c r="F58" s="132"/>
+      <c r="G58" s="132"/>
+      <c r="H58" s="132"/>
+      <c r="I58" s="132"/>
+      <c r="J58" s="132"/>
+      <c r="K58" s="132"/>
+      <c r="L58" s="132"/>
+      <c r="M58" s="132"/>
     </row>
     <row r="59" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="18">
         <v>3.1</v>
       </c>
-      <c r="B59" s="115" t="s">
+      <c r="B59" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="115"/>
-      <c r="D59" s="115"/>
-      <c r="E59" s="115"/>
-      <c r="F59" s="115"/>
-      <c r="G59" s="115"/>
-      <c r="H59" s="115"/>
-      <c r="I59" s="115"/>
-      <c r="J59" s="115"/>
-      <c r="K59" s="115"/>
-      <c r="L59" s="115"/>
-      <c r="M59" s="115"/>
+      <c r="C59" s="127"/>
+      <c r="D59" s="127"/>
+      <c r="E59" s="127"/>
+      <c r="F59" s="127"/>
+      <c r="G59" s="127"/>
+      <c r="H59" s="127"/>
+      <c r="I59" s="127"/>
+      <c r="J59" s="127"/>
+      <c r="K59" s="127"/>
+      <c r="L59" s="127"/>
+      <c r="M59" s="127"/>
     </row>
     <row r="60" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="116" t="s">
+      <c r="B60" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="C60" s="117"/>
-      <c r="D60" s="118"/>
-      <c r="E60" s="116" t="s">
+      <c r="C60" s="118"/>
+      <c r="D60" s="119"/>
+      <c r="E60" s="117" t="s">
         <v>96</v>
       </c>
-      <c r="F60" s="117"/>
-      <c r="G60" s="118"/>
-      <c r="H60" s="116"/>
-      <c r="I60" s="117"/>
-      <c r="J60" s="117"/>
-      <c r="K60" s="118"/>
+      <c r="F60" s="118"/>
+      <c r="G60" s="119"/>
+      <c r="H60" s="117"/>
+      <c r="I60" s="118"/>
+      <c r="J60" s="118"/>
+      <c r="K60" s="119"/>
       <c r="L60" s="33"/>
       <c r="M60" s="33"/>
     </row>
@@ -4309,39 +4313,39 @@
       <c r="A61" s="18">
         <v>3.2</v>
       </c>
-      <c r="B61" s="115" t="s">
+      <c r="B61" s="127" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="115"/>
-      <c r="D61" s="115"/>
-      <c r="E61" s="115"/>
-      <c r="F61" s="115"/>
-      <c r="G61" s="115"/>
-      <c r="H61" s="115"/>
-      <c r="I61" s="115"/>
-      <c r="J61" s="115"/>
-      <c r="K61" s="115"/>
-      <c r="L61" s="115"/>
-      <c r="M61" s="115"/>
+      <c r="C61" s="127"/>
+      <c r="D61" s="127"/>
+      <c r="E61" s="127"/>
+      <c r="F61" s="127"/>
+      <c r="G61" s="127"/>
+      <c r="H61" s="127"/>
+      <c r="I61" s="127"/>
+      <c r="J61" s="127"/>
+      <c r="K61" s="127"/>
+      <c r="L61" s="127"/>
+      <c r="M61" s="127"/>
     </row>
     <row r="62" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="116" t="s">
+      <c r="B62" s="117" t="s">
         <v>95</v>
       </c>
-      <c r="C62" s="117"/>
-      <c r="D62" s="118"/>
-      <c r="E62" s="116" t="s">
+      <c r="C62" s="118"/>
+      <c r="D62" s="119"/>
+      <c r="E62" s="117" t="s">
         <v>97</v>
       </c>
-      <c r="F62" s="117"/>
-      <c r="G62" s="118"/>
-      <c r="H62" s="116"/>
-      <c r="I62" s="117"/>
-      <c r="J62" s="117"/>
-      <c r="K62" s="118"/>
+      <c r="F62" s="118"/>
+      <c r="G62" s="119"/>
+      <c r="H62" s="117"/>
+      <c r="I62" s="118"/>
+      <c r="J62" s="118"/>
+      <c r="K62" s="119"/>
       <c r="L62" s="33"/>
       <c r="M62" s="33"/>
     </row>
@@ -4349,39 +4353,39 @@
       <c r="A63" s="18">
         <v>3.3</v>
       </c>
-      <c r="B63" s="115" t="s">
+      <c r="B63" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="115"/>
-      <c r="D63" s="115"/>
-      <c r="E63" s="115"/>
-      <c r="F63" s="115"/>
-      <c r="G63" s="115"/>
-      <c r="H63" s="115"/>
-      <c r="I63" s="115"/>
-      <c r="J63" s="115"/>
-      <c r="K63" s="115"/>
-      <c r="L63" s="115"/>
-      <c r="M63" s="115"/>
+      <c r="C63" s="127"/>
+      <c r="D63" s="127"/>
+      <c r="E63" s="127"/>
+      <c r="F63" s="127"/>
+      <c r="G63" s="127"/>
+      <c r="H63" s="127"/>
+      <c r="I63" s="127"/>
+      <c r="J63" s="127"/>
+      <c r="K63" s="127"/>
+      <c r="L63" s="127"/>
+      <c r="M63" s="127"/>
     </row>
     <row r="64" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="116" t="s">
+      <c r="B64" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="117"/>
-      <c r="D64" s="118"/>
-      <c r="E64" s="116" t="s">
+      <c r="C64" s="118"/>
+      <c r="D64" s="119"/>
+      <c r="E64" s="117" t="s">
         <v>96</v>
       </c>
-      <c r="F64" s="117"/>
-      <c r="G64" s="118"/>
-      <c r="H64" s="116"/>
-      <c r="I64" s="117"/>
-      <c r="J64" s="117"/>
-      <c r="K64" s="118"/>
+      <c r="F64" s="118"/>
+      <c r="G64" s="119"/>
+      <c r="H64" s="117"/>
+      <c r="I64" s="118"/>
+      <c r="J64" s="118"/>
+      <c r="K64" s="119"/>
       <c r="L64" s="33"/>
       <c r="M64" s="33"/>
     </row>
@@ -4389,20 +4393,20 @@
       <c r="A65" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="116" t="s">
+      <c r="B65" s="117" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="117"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="116" t="s">
+      <c r="C65" s="118"/>
+      <c r="D65" s="119"/>
+      <c r="E65" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="F65" s="117"/>
-      <c r="G65" s="118"/>
-      <c r="H65" s="116"/>
-      <c r="I65" s="117"/>
-      <c r="J65" s="117"/>
-      <c r="K65" s="118"/>
+      <c r="F65" s="118"/>
+      <c r="G65" s="119"/>
+      <c r="H65" s="117"/>
+      <c r="I65" s="118"/>
+      <c r="J65" s="118"/>
+      <c r="K65" s="119"/>
       <c r="L65" s="40"/>
       <c r="M65" s="40"/>
     </row>
@@ -4410,41 +4414,41 @@
       <c r="A66" s="18">
         <v>4</v>
       </c>
-      <c r="B66" s="118" t="s">
+      <c r="B66" s="119" t="s">
         <v>167</v>
       </c>
-      <c r="C66" s="115"/>
-      <c r="D66" s="115"/>
-      <c r="E66" s="115"/>
-      <c r="F66" s="115"/>
-      <c r="G66" s="115"/>
-      <c r="H66" s="115"/>
-      <c r="I66" s="115"/>
-      <c r="J66" s="115"/>
-      <c r="K66" s="115"/>
-      <c r="L66" s="115"/>
-      <c r="M66" s="115"/>
+      <c r="C66" s="127"/>
+      <c r="D66" s="127"/>
+      <c r="E66" s="127"/>
+      <c r="F66" s="127"/>
+      <c r="G66" s="127"/>
+      <c r="H66" s="127"/>
+      <c r="I66" s="127"/>
+      <c r="J66" s="127"/>
+      <c r="K66" s="127"/>
+      <c r="L66" s="127"/>
+      <c r="M66" s="127"/>
     </row>
     <row r="67" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B67" s="116" t="s">
+      <c r="B67" s="117" t="s">
         <v>170</v>
       </c>
-      <c r="C67" s="117"/>
-      <c r="D67" s="118"/>
-      <c r="E67" s="116" t="s">
+      <c r="C67" s="118"/>
+      <c r="D67" s="119"/>
+      <c r="E67" s="117" t="s">
         <v>168</v>
       </c>
-      <c r="F67" s="117"/>
-      <c r="G67" s="118"/>
-      <c r="H67" s="116" t="s">
+      <c r="F67" s="118"/>
+      <c r="G67" s="119"/>
+      <c r="H67" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="I67" s="124"/>
-      <c r="J67" s="124"/>
-      <c r="K67" s="125"/>
+      <c r="I67" s="125"/>
+      <c r="J67" s="125"/>
+      <c r="K67" s="126"/>
       <c r="L67" s="42"/>
       <c r="M67" s="41"/>
     </row>
@@ -4452,22 +4456,22 @@
       <c r="A68" s="18">
         <v>4.2</v>
       </c>
-      <c r="B68" s="126" t="s">
+      <c r="B68" s="123" t="s">
         <v>171</v>
       </c>
-      <c r="C68" s="127"/>
-      <c r="D68" s="128"/>
-      <c r="E68" s="126" t="s">
+      <c r="C68" s="120"/>
+      <c r="D68" s="124"/>
+      <c r="E68" s="123" t="s">
         <v>168</v>
       </c>
-      <c r="F68" s="127"/>
-      <c r="G68" s="128"/>
-      <c r="H68" s="116" t="s">
+      <c r="F68" s="120"/>
+      <c r="G68" s="124"/>
+      <c r="H68" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="I68" s="124"/>
-      <c r="J68" s="124"/>
-      <c r="K68" s="125"/>
+      <c r="I68" s="125"/>
+      <c r="J68" s="125"/>
+      <c r="K68" s="126"/>
       <c r="L68" s="42"/>
       <c r="M68" s="41"/>
     </row>
@@ -4475,22 +4479,22 @@
       <c r="A69" s="18">
         <v>4.3</v>
       </c>
-      <c r="B69" s="129" t="s">
+      <c r="B69" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="C69" s="130"/>
-      <c r="D69" s="131"/>
-      <c r="E69" s="126" t="s">
+      <c r="C69" s="115"/>
+      <c r="D69" s="116"/>
+      <c r="E69" s="123" t="s">
         <v>168</v>
       </c>
-      <c r="F69" s="127"/>
-      <c r="G69" s="128"/>
-      <c r="H69" s="116" t="s">
+      <c r="F69" s="120"/>
+      <c r="G69" s="124"/>
+      <c r="H69" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="I69" s="124"/>
-      <c r="J69" s="124"/>
-      <c r="K69" s="125"/>
+      <c r="I69" s="125"/>
+      <c r="J69" s="125"/>
+      <c r="K69" s="126"/>
       <c r="L69" s="42"/>
       <c r="M69" s="41"/>
     </row>
@@ -4498,22 +4502,22 @@
       <c r="A70" s="18">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B70" s="129" t="s">
+      <c r="B70" s="114" t="s">
         <v>173</v>
       </c>
-      <c r="C70" s="130"/>
-      <c r="D70" s="131"/>
-      <c r="E70" s="126" t="s">
+      <c r="C70" s="115"/>
+      <c r="D70" s="116"/>
+      <c r="E70" s="123" t="s">
         <v>168</v>
       </c>
-      <c r="F70" s="127"/>
-      <c r="G70" s="128"/>
-      <c r="H70" s="116" t="s">
+      <c r="F70" s="120"/>
+      <c r="G70" s="124"/>
+      <c r="H70" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="I70" s="124"/>
-      <c r="J70" s="124"/>
-      <c r="K70" s="125"/>
+      <c r="I70" s="125"/>
+      <c r="J70" s="125"/>
+      <c r="K70" s="126"/>
       <c r="L70" s="42"/>
       <c r="M70" s="41"/>
     </row>
@@ -4521,22 +4525,22 @@
       <c r="A71" s="18">
         <v>4.5</v>
       </c>
-      <c r="B71" s="126" t="s">
+      <c r="B71" s="123" t="s">
         <v>174</v>
       </c>
-      <c r="C71" s="127"/>
-      <c r="D71" s="128"/>
-      <c r="E71" s="116" t="s">
+      <c r="C71" s="120"/>
+      <c r="D71" s="124"/>
+      <c r="E71" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="F71" s="117"/>
-      <c r="G71" s="118"/>
-      <c r="H71" s="126" t="s">
+      <c r="F71" s="118"/>
+      <c r="G71" s="119"/>
+      <c r="H71" s="123" t="s">
         <v>178</v>
       </c>
-      <c r="I71" s="132"/>
-      <c r="J71" s="132"/>
-      <c r="K71" s="133"/>
+      <c r="I71" s="121"/>
+      <c r="J71" s="121"/>
+      <c r="K71" s="122"/>
       <c r="L71" s="42"/>
       <c r="M71" s="41"/>
     </row>
@@ -4544,22 +4548,22 @@
       <c r="A72" s="18">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B72" s="116" t="s">
+      <c r="B72" s="117" t="s">
         <v>175</v>
       </c>
-      <c r="C72" s="117"/>
-      <c r="D72" s="118"/>
-      <c r="E72" s="116" t="s">
+      <c r="C72" s="118"/>
+      <c r="D72" s="119"/>
+      <c r="E72" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="F72" s="117"/>
-      <c r="G72" s="118"/>
-      <c r="H72" s="127" t="s">
+      <c r="F72" s="118"/>
+      <c r="G72" s="119"/>
+      <c r="H72" s="120" t="s">
         <v>178</v>
       </c>
-      <c r="I72" s="132"/>
-      <c r="J72" s="132"/>
-      <c r="K72" s="133"/>
+      <c r="I72" s="121"/>
+      <c r="J72" s="121"/>
+      <c r="K72" s="122"/>
       <c r="L72" s="42"/>
       <c r="M72" s="41"/>
     </row>
@@ -4567,22 +4571,22 @@
       <c r="A73" s="18">
         <v>4.7</v>
       </c>
-      <c r="B73" s="129" t="s">
+      <c r="B73" s="114" t="s">
         <v>176</v>
       </c>
-      <c r="C73" s="130"/>
-      <c r="D73" s="131"/>
-      <c r="E73" s="116" t="s">
+      <c r="C73" s="115"/>
+      <c r="D73" s="116"/>
+      <c r="E73" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="F73" s="117"/>
-      <c r="G73" s="118"/>
-      <c r="H73" s="127" t="s">
+      <c r="F73" s="118"/>
+      <c r="G73" s="119"/>
+      <c r="H73" s="120" t="s">
         <v>178</v>
       </c>
-      <c r="I73" s="132"/>
-      <c r="J73" s="132"/>
-      <c r="K73" s="133"/>
+      <c r="I73" s="121"/>
+      <c r="J73" s="121"/>
+      <c r="K73" s="122"/>
       <c r="L73" s="42"/>
       <c r="M73" s="41"/>
     </row>
@@ -4590,22 +4594,22 @@
       <c r="A74" s="18">
         <v>4.8</v>
       </c>
-      <c r="B74" s="129" t="s">
+      <c r="B74" s="114" t="s">
         <v>175</v>
       </c>
-      <c r="C74" s="130"/>
-      <c r="D74" s="131"/>
-      <c r="E74" s="126" t="s">
+      <c r="C74" s="115"/>
+      <c r="D74" s="116"/>
+      <c r="E74" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="F74" s="127"/>
-      <c r="G74" s="128"/>
-      <c r="H74" s="127" t="s">
+      <c r="F74" s="120"/>
+      <c r="G74" s="124"/>
+      <c r="H74" s="120" t="s">
         <v>178</v>
       </c>
-      <c r="I74" s="132"/>
-      <c r="J74" s="132"/>
-      <c r="K74" s="133"/>
+      <c r="I74" s="121"/>
+      <c r="J74" s="121"/>
+      <c r="K74" s="122"/>
       <c r="L74" s="42"/>
       <c r="M74" s="41"/>
     </row>
@@ -4626,31 +4630,133 @@
     </row>
   </sheetData>
   <mergeCells count="176">
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="H71:K71"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="B66:M66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="H67:K67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="H68:K68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B59:M59"/>
+    <mergeCell ref="B61:M61"/>
+    <mergeCell ref="B63:M63"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="B58:M58"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B42:M42"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="B50:M50"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="H62:K62"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:K26"/>
     <mergeCell ref="H57:K57"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="E47:G47"/>
@@ -4675,133 +4781,31 @@
     <mergeCell ref="H48:K48"/>
     <mergeCell ref="H49:K49"/>
     <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="H62:K62"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="B50:M50"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B42:M42"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="B59:M59"/>
-    <mergeCell ref="B61:M61"/>
-    <mergeCell ref="B63:M63"/>
-    <mergeCell ref="B10:M10"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="B58:M58"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B66:M66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="H67:K67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="H68:K68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="H71:K71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="H72:K72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>